<commit_message>
Fixes to custom commands and added new ones to help with loading initial data
</commit_message>
<xml_diff>
--- a/fg/external_files/players.xlsx
+++ b/fg/external_files/players.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexevans/Desktop/Projects/fgolf/fg/external_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexevans/Library/Containers/com.microsoft.Excel/Data/Desktop/Projects/fgolf/fg/external_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4B71C70F-96DC-224E-A587-F698F255B9AC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{108924EB-F1A9-6C4A-9297-9303A52FADE4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="15920" xr2:uid="{11440A6E-CB72-CD4F-877F-52107475F245}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="266">
   <si>
     <t>PLAYER NAME</t>
   </si>
@@ -823,6 +823,12 @@
   </si>
   <si>
     <t>Will MacKenzie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thorbjorn Olesen </t>
+  </si>
+  <si>
+    <t>Erik van Rooyen</t>
   </si>
 </sst>
 </file>
@@ -873,10 +879,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1192,1602 +1199,2409 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D41022FE-CC28-3440-96D2-01DB4AC39B52}">
-  <dimension ref="A1:A264"/>
+  <dimension ref="A1:B266"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A248" workbookViewId="0">
+      <selection activeCell="E270" sqref="E270"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.6640625" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="2" max="2" width="25.6640625" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="20" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2" ht="20" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B3" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B4" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B5" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B6" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B7" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B8" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B9" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B10" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B11" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B12" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B13" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B14" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B15" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B16" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B17" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B18" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B19" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B20" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B21" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B22" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B23" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B24" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B25" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B26" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B27" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B28" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B29" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B30" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B31" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B32" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B33" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B34" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B35" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B36" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B37" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B38" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B39" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B40" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B41" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B42" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B43" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B44" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B45" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B46" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B47" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B48" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B49" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B50" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B51" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B52" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B53" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B54" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B55" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B56" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B57" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B58" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B59" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B60" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B61" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B62" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B63" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B64" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B65" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B66" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B67" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B68" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B69" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B70" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B71" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B72" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B73" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B74" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B75" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B76" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B77" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B78" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B79" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B80" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B81" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B82" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B83" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B84" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B85" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B86" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B87" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B88" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B89" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B90" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B91" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B92" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B93" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B94" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B95" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B96" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B97" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B98" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B99" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B100" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B101" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B102" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B103" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104" s="2" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B104" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B105" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106" s="2" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B106" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B107" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B108" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109" s="2" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B109" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110" s="2" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B110" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B111" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A112" s="2" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B112" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A113" s="2" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B113" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B114" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B115" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116" s="2" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B116" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A117" s="2" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B117" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A118" s="2" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B118" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A119" s="2" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B119" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A120" s="2" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B120" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A121" s="2" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B121" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A122" s="2" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B122" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A123" s="2" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B123" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A124" s="2" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B124" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A125" s="2" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B125" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A126" s="2" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B126" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A127" s="2" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B127" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A128" s="2" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B128" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A129" s="2" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B129" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A130" s="2" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B130" s="3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A131" s="2" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B131" s="3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A132" s="2" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B132" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A133" s="2" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B133" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A134" s="2" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B134" s="3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A135" s="2" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B135" s="3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A136" s="2" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B136" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A137" s="2" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B137" s="3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A138" s="2" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B138" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A139" s="2" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B139" s="3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A140" s="2" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B140" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A141" s="2" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B141" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A142" s="2" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B142" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A143" s="2" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B143" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A144" s="2" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B144" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A145" s="2" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B145" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A146" s="2" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B146" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A147" s="2" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B147" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A148" s="2" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B148" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A149" s="2" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B149" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A150" s="2" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B150" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A151" s="2" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B151" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A152" s="2" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B152" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A153" s="2" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B153" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A154" s="2" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B154" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A155" s="2" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B155" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A156" s="2" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B156" s="3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A157" s="2" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B157" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A158" s="2" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B158" s="3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A159" s="2" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B159" s="3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A160" s="2" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B160" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A161" s="2" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B161" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A162" s="2" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B162" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A163" s="2" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B163" s="3" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A164" s="2" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B164" s="3" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A165" s="2" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B165" s="3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A166" s="2" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B166" s="3" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A167" s="2" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B167" s="3" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A168" s="2" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B168" s="3" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A169" s="2" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B169" s="3" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A170" s="2" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B170" s="3" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A171" s="2" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B171" s="3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A172" s="2" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B172" s="3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A173" s="2" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B173" s="3" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A174" s="2" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B174" s="3" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A175" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B175" s="3" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A176" s="2" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B176" s="3" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A177" s="2" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B177" s="3" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A178" s="2" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B178" s="3" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A179" s="2" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B179" s="3" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A180" s="2" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B180" s="3" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A181" s="2" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B181" s="3" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A182" s="2" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B182" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A183" s="2" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B183" s="3" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A184" s="2" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B184" s="3" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A185" s="2" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B185" s="3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A186" s="2" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B186" s="3" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A187" s="2" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B187" s="3" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A188" s="2" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B188" s="3" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A189" s="2" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B189" s="3" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A190" s="2" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B190" s="3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A191" s="2" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B191" s="3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A192" s="2" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B192" s="3" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A193" s="2" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B193" s="3" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A194" s="2" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B194" s="3" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A195" s="2" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B195" s="3" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A196" s="2" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B196" s="3" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A197" s="2" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B197" s="3" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A198" s="2" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B198" s="3" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A199" s="2" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B199" s="3" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A200" s="2" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B200" s="3" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A201" s="2" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B201" s="3" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A202" s="2" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B202" s="3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A203" s="2" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B203" s="3" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A204" s="2" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B204" s="3" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A205" s="2" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B205" s="3" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A206" s="2" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B206" s="3" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A207" s="2" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B207" s="3" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A208" s="2" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B208" s="3" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A209" s="2" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B209" s="3" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A210" s="2" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="211" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B210" s="3" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A211" s="2" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="212" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B211" s="3" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A212" s="2" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="213" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B212" s="3" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A213" s="2" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="214" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B213" s="3" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A214" s="2" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="215" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B214" s="3" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A215" s="2" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="216" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B215" s="3" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A216" s="2" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="217" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B216" s="3" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A217" s="2" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="218" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B217" s="3" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A218" s="2" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="219" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B218" s="3" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A219" s="2" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="220" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B219" s="3" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A220" s="2" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="221" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B220" s="3" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A221" s="2" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="222" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B221" s="3" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A222" s="2" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="223" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B222" s="3" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A223" s="2" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="224" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B223" s="3" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A224" s="2" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="225" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B224" s="3" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A225" s="2" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="226" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B225" s="3" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A226" s="2" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="227" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B226" s="3" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A227" s="2" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="228" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B227" s="3" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A228" s="2" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="229" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B228" s="3" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A229" s="2" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="230" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B229" s="3" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A230" s="2" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="231" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B230" s="3" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A231" s="2" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="232" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B231" s="3" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A232" s="2" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="233" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B232" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A233" s="2" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="234" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B233" s="3" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A234" s="2" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="235" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B234" s="3" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A235" s="2" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="236" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B235" s="3" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A236" s="2" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="237" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B236" s="3" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A237" s="2" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="238" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B237" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A238" s="2" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="239" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B238" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A239" s="2" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="240" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B239" s="3" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A240" s="2" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="241" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B240" s="3" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A241" s="2" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="242" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B241" s="3" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A242" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="243" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B242" s="3" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A243" s="2" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="244" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B243" s="3" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A244" s="2" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="245" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B244" s="3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A245" s="2" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="246" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B245" s="3" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A246" s="2" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="247" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B246" s="3" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A247" s="2" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="248" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B247" s="3" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A248" s="2" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="249" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B248" s="3" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A249" s="2" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="250" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B249" s="3" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A250" s="2" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="251" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B250" s="3" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A251" s="2" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="252" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B251" s="3" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A252" s="2" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="253" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B252" s="3" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A253" s="2" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="254" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B253" s="3" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A254" s="2" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="255" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B254" s="3" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A255" s="2" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="256" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B255" s="3" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A256" s="2" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="257" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B256" s="3" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A257" s="2" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="258" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B257" s="3" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A258" s="2" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="259" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B258" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A259" s="2" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="260" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B259" s="3" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A260" s="2" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="261" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B260" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A261" s="2" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="262" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B261" s="3" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A262" s="2" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="263" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B262" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A263" s="2" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="264" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B263" s="3" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A264" s="2" t="s">
         <v>263</v>
       </c>
+      <c r="B264" s="3" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A265" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="B265" s="2" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A266" s="2" t="s">
+        <v>265</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://www.pgatour.com/players/player.36689.brooks-koepka.html" xr:uid="{19C38C8B-3103-114E-9601-BF899EAB67EC}"/>
-    <hyperlink ref="A3" r:id="rId2" display="https://www.pgatour.com/players/player.23108.matt-kuchar.html" xr:uid="{0A4CDD65-52B4-DF42-9ACC-E54F234DB6EB}"/>
-    <hyperlink ref="A4" r:id="rId3" display="https://www.pgatour.com/players/player.28237.rory-mcilroy.html" xr:uid="{05DC64AE-5124-F443-BD24-AE18EA5D9D72}"/>
-    <hyperlink ref="A5" r:id="rId4" display="https://www.pgatour.com/players/player.48081.xander-schauffele.html" xr:uid="{D423EAFF-3DEA-F941-A0C5-D6C00DFBB273}"/>
-    <hyperlink ref="A6" r:id="rId5" display="https://www.pgatour.com/players/player.31323.gary-woodland.html" xr:uid="{318440CC-F733-BE44-91DA-E71EE4F410A5}"/>
-    <hyperlink ref="A7" r:id="rId6" display="https://www.pgatour.com/players/player.35450.patrick-cantlay.html" xr:uid="{3E7E195E-82EE-1B48-83C7-28C85EB1BA54}"/>
-    <hyperlink ref="A8" r:id="rId7" display="https://www.pgatour.com/players/player.30925.dustin-johnson.html" xr:uid="{07036675-2AA5-214D-AEFF-915EC3F4193B}"/>
-    <hyperlink ref="A9" r:id="rId8" display="https://www.pgatour.com/players/player.25364.paul-casey.html" xr:uid="{29EC0822-DBD2-7E48-B6F6-D77EA29652EC}"/>
-    <hyperlink ref="A10" r:id="rId9" display="https://www.pgatour.com/players/player.32102.rickie-fowler.html" xr:uid="{3535F1EB-6895-0F4C-AD8E-AE75EDCFFB25}"/>
-    <hyperlink ref="A11" r:id="rId10" display="https://www.pgatour.com/players/player.46970.jon-rahm.html" xr:uid="{116BF79F-71F0-E848-BA60-CDC4C378B9A6}"/>
-    <hyperlink ref="A12" r:id="rId11" display="https://www.pgatour.com/players/player.22405.justin-rose.html" xr:uid="{256E6740-6035-4A4C-9797-E2855D43D6F7}"/>
-    <hyperlink ref="A13" r:id="rId12" display="https://www.pgatour.com/players/player.26476.chez-reavie.html" xr:uid="{F35ED584-EFB4-6347-AB43-0C7CB91F7DB5}"/>
-    <hyperlink ref="A14" r:id="rId13" display="https://www.pgatour.com/players/player.29725.tony-finau.html" xr:uid="{64630654-D22B-3744-A0F0-7305104C43E4}"/>
-    <hyperlink ref="A15" r:id="rId14" display="https://www.pgatour.com/players/player.21961.charles-howell-iii.html" xr:uid="{F32B9834-CD0D-384A-AE3A-70AB23CD722D}"/>
-    <hyperlink ref="A16" r:id="rId15" display="https://www.pgatour.com/players/player.26851.marc-leishman.html" xr:uid="{6A246AC7-A653-234F-9249-EC39504D1817}"/>
-    <hyperlink ref="A17" r:id="rId16" display="https://www.pgatour.com/players/player.47959.bryson-dechambeau.html" xr:uid="{ADF423C5-588D-7846-96B4-C063874213E5}"/>
-    <hyperlink ref="A18" r:id="rId17" display="https://www.pgatour.com/players/player.33448.justin-thomas.html" xr:uid="{BF0C1BFB-4105-9443-AE35-F47CC68CCD36}"/>
-    <hyperlink ref="A19" r:id="rId18" display="https://www.pgatour.com/players/player.33204.shane-lowry.html" xr:uid="{83493519-8AC8-FD43-B749-E884F14A0B8D}"/>
-    <hyperlink ref="A20" r:id="rId19" display="https://www.pgatour.com/players/player.24502.adam-scott.html" xr:uid="{57EFA7F9-0B05-1B46-A54D-60D1FC01F1B1}"/>
-    <hyperlink ref="A21" r:id="rId20" display="https://www.pgatour.com/players/player.30911.tommy-fleetwood.html" xr:uid="{923E6B3F-AF64-1841-A47F-DDB7607323AF}"/>
-    <hyperlink ref="A22" r:id="rId21" display="https://www.pgatour.com/players/player.29478.kevin-kisner.html" xr:uid="{C9AD37E9-6800-A041-99A7-0EBA64A72439}"/>
-    <hyperlink ref="A23" r:id="rId22" display="https://www.pgatour.com/players/player.25198.francesco-molinari.html" xr:uid="{56AAADC5-B275-8942-B721-6B8A7CDFC739}"/>
-    <hyperlink ref="A24" r:id="rId23" display="https://www.pgatour.com/players/player.23320.ryan-palmer.html" xr:uid="{DE1D17B6-9C1B-FC40-BDA0-06FF8D34310E}"/>
-    <hyperlink ref="A25" r:id="rId24" display="https://www.pgatour.com/players/player.39971.sungjae-im.html" xr:uid="{DE51F83D-09C8-804E-8759-41384AE6AC3F}"/>
-    <hyperlink ref="A26" r:id="rId25" display="https://www.pgatour.com/players/player.25818.scott-piercy.html" xr:uid="{64D9376B-4634-4E40-9081-A33C08A0AAB8}"/>
-    <hyperlink ref="A27" r:id="rId26" display="https://www.pgatour.com/players/player.29221.webb-simpson.html" xr:uid="{8E1585C0-FED8-524E-BB2D-6D95A8E0A9DA}"/>
-    <hyperlink ref="A28" r:id="rId27" display="https://www.pgatour.com/players/player.08793.tiger-woods.html" xr:uid="{C8ECA2A8-0CD2-284F-B67B-A7A3B94D6979}"/>
-    <hyperlink ref="A29" r:id="rId28" display="https://www.pgatour.com/players/player.27974.sung-kang.html" xr:uid="{0E618548-6B6C-5647-9687-4E72347662E4}"/>
-    <hyperlink ref="A30" r:id="rId29" display="https://www.pgatour.com/players/player.32839.hideki-matsuyama.html" xr:uid="{D4F4F67A-CB3D-0C4C-861F-778C58A599E2}"/>
-    <hyperlink ref="A31" r:id="rId30" display="https://www.pgatour.com/players/player.25900.lucas-glover.html" xr:uid="{EFD2F0CC-C34E-4D45-B1DF-51D0D7D569FF}"/>
-    <hyperlink ref="A32" r:id="rId31" display="https://www.pgatour.com/players/player.39997.corey-conners.html" xr:uid="{BF259E64-2493-2542-A0AE-8F503770F7C5}"/>
-    <hyperlink ref="A33" r:id="rId32" display="https://www.pgatour.com/players/player.01810.phil-mickelson.html" xr:uid="{18D0B03F-C8DA-704C-BB55-41A65F4A050B}"/>
-    <hyperlink ref="A34" r:id="rId33" display="https://www.pgatour.com/players/player.27649.brandt-snedeker.html" xr:uid="{AC63956D-C55D-084A-8C7F-4E0CF3262E25}"/>
-    <hyperlink ref="A35" r:id="rId34" display="https://www.pgatour.com/players/player.29908.c-t--pan.html" xr:uid="{5D2BE600-EBFD-784B-8AA6-9B1DB9C6FB3E}"/>
-    <hyperlink ref="A36" r:id="rId35" display="https://www.pgatour.com/players/player.39546.keith-mitchell.html" xr:uid="{68D45301-295D-0D4E-99E2-46B5E427FEC7}"/>
-    <hyperlink ref="A37" r:id="rId36" display="https://www.pgatour.com/players/player.32333.kevin-tway.html" xr:uid="{FE9D87DC-564D-D94C-BAE0-666FE1E0AFB2}"/>
-    <hyperlink ref="A38" r:id="rId37" display="https://www.pgatour.com/players/player.28089.jason-day.html" xr:uid="{ED832C2F-500C-154A-8BDE-A6E1D3E19424}"/>
-    <hyperlink ref="A39" r:id="rId38" display="https://www.pgatour.com/players/player.10809.jim-furyk.html" xr:uid="{3E9EEF53-0830-E346-9CD1-E189D3C160D5}"/>
-    <hyperlink ref="A40" r:id="rId39" display="https://www.pgatour.com/players/player.34256.andrew-putnam.html" xr:uid="{6B856F7A-F281-B242-A096-7AC579C3D0E2}"/>
-    <hyperlink ref="A41" r:id="rId40" display="https://www.pgatour.com/players/player.33399.adam-hadwin.html" xr:uid="{0D9B5423-0914-964C-B2B5-B5F1C680EB94}"/>
-    <hyperlink ref="A42" r:id="rId41" display="https://www.pgatour.com/players/player.23621.rory-sabbatini.html" xr:uid="{DD8C1E76-D4B0-1347-A3BF-EB3224562383}"/>
-    <hyperlink ref="A43" r:id="rId42" display="https://www.pgatour.com/players/player.27141.j-b--holmes.html" xr:uid="{6D5882D0-D6E1-5A47-93EE-225AC718E26F}"/>
-    <hyperlink ref="A44" r:id="rId43" display="https://www.pgatour.com/players/player.25396.kevin-na.html" xr:uid="{919283EA-2DB9-7042-84C7-51FFFFF13914}"/>
-    <hyperlink ref="A45" r:id="rId44" display="https://www.pgatour.com/players/player.28775.nate-lashley.html" xr:uid="{DFF8CF59-4988-4242-AE09-183289B2D535}"/>
-    <hyperlink ref="A46" r:id="rId45" display="https://www.pgatour.com/players/player.30944.jason-kokrak.html" xr:uid="{C64B7A10-4DCB-3A49-A296-98FF460231B3}"/>
-    <hyperlink ref="A47" r:id="rId46" display="https://www.pgatour.com/players/player.39977.max-homa.html" xr:uid="{FB46DC0C-A28E-9C45-AEF7-589102633509}"/>
-    <hyperlink ref="A48" r:id="rId47" display="https://www.pgatour.com/players/player.29970.dylan-frittelli.html" xr:uid="{9E084D34-E587-5542-B3CB-895BF7F2DE71}"/>
-    <hyperlink ref="A49" r:id="rId48" display="https://www.pgatour.com/players/player.25572.graeme-mcdowell.html" xr:uid="{A0E1FCFA-047A-C545-99D1-4FCBBFC91299}"/>
-    <hyperlink ref="A50" r:id="rId49" display="https://www.pgatour.com/players/player.37455.si-woo-kim.html" xr:uid="{BD5F44E3-AF8F-4C48-A24B-5123CFD85306}"/>
-    <hyperlink ref="A51" r:id="rId50" display="https://www.pgatour.com/players/player.34076.joel-dahmen.html" xr:uid="{540FCE23-A3D0-CE41-BE59-8A57E5621190}"/>
-    <hyperlink ref="A52" r:id="rId51" display="https://www.pgatour.com/players/player.26329.louis-oosthuizen.html" xr:uid="{62D1AB31-8DCB-C84B-8183-88B00F431176}"/>
-    <hyperlink ref="A53" r:id="rId52" display="https://www.pgatour.com/players/player.33141.keegan-bradley.html" xr:uid="{12037586-18D8-A649-8591-3AE29A0EC404}"/>
-    <hyperlink ref="A54" r:id="rId53" display="https://www.pgatour.com/players/player.26596.ryan-moore.html" xr:uid="{8C7FCF59-5698-A649-9086-0AB029E75E58}"/>
-    <hyperlink ref="A55" r:id="rId54" display="https://www.pgatour.com/players/player.34360.patrick-reed.html" xr:uid="{36F3CD31-2FC4-6A45-B105-E19F6EC71395}"/>
-    <hyperlink ref="A56" r:id="rId55" display="https://www.pgatour.com/players/player.35449.adam-long.html" xr:uid="{E57CBF0B-A982-4641-A3FC-68420065136C}"/>
-    <hyperlink ref="A57" r:id="rId56" display="https://www.pgatour.com/players/player.29420.billy-horschel.html" xr:uid="{31E142A1-BC15-774B-95CC-345F554D7AD1}"/>
-    <hyperlink ref="A58" r:id="rId57" display="https://www.pgatour.com/players/player.31646.emiliano-grillo.html" xr:uid="{5CFBC3E3-A5B1-8F4B-AD3D-7DD0339C72AD}"/>
-    <hyperlink ref="A59" r:id="rId58" display="https://www.pgatour.com/players/player.52372.cameron-champ.html" xr:uid="{7A42E780-FF7D-F445-AE97-17B6DEFCD001}"/>
-    <hyperlink ref="A60" r:id="rId59" display="https://www.pgatour.com/players/player.26499.rafa-cabrera-bello.html" xr:uid="{B8B77CCE-43D8-1345-A9AA-F5CC7DF32FA5}"/>
-    <hyperlink ref="A61" r:id="rId60" display="https://www.pgatour.com/players/player.23325.vaughn-taylor.html" xr:uid="{2D3F4061-C2E1-454A-B6B5-36CB18A81598}"/>
-    <hyperlink ref="A62" r:id="rId61" display="https://www.pgatour.com/players/player.29926.danny-lee.html" xr:uid="{3ABA9150-8F3A-9044-BF03-958BC80FCFAF}"/>
-    <hyperlink ref="A63" r:id="rId62" display="https://www.pgatour.com/players/player.45526.abraham-ancer.html" xr:uid="{21850AA5-24AD-C148-9E8C-9B567AFE8C4C}"/>
-    <hyperlink ref="A64" r:id="rId63" display="https://www.pgatour.com/players/player.21209.sergio-garcia.html" xr:uid="{DF7A5EBA-A52F-434D-ADAE-2694BBE0E987}"/>
-    <hyperlink ref="A65" r:id="rId64" display="https://www.pgatour.com/players/player.27214.kevin-streelman.html" xr:uid="{6FA7833D-CF23-AA40-9C77-039F20B5123A}"/>
-    <hyperlink ref="A66" r:id="rId65" display="https://www.pgatour.com/players/player.24138.ian-poulter.html" xr:uid="{7575D5CC-8DC6-4C44-807B-267A883C5DF6}"/>
-    <hyperlink ref="A67" r:id="rId66" display="https://www.pgatour.com/players/player.12716.charley-hoffman.html" xr:uid="{B2481BDB-BF71-1840-B313-FFE0DF90C38A}"/>
-    <hyperlink ref="A68" r:id="rId67" display="https://www.pgatour.com/players/player.30978.kiradech-aphibarnrat.html" xr:uid="{9EF35A78-79D8-824E-BB9A-C529DA9F79C3}"/>
-    <hyperlink ref="A69" r:id="rId68" display="https://www.pgatour.com/players/player.28307.matt-every.html" xr:uid="{49416DBC-B59B-2149-BDD0-CD2BC246036A}"/>
-    <hyperlink ref="A70" r:id="rId69" display="https://www.pgatour.com/players/player.34046.jordan-spieth.html" xr:uid="{1F1301CC-4953-B44B-81C4-C5C8364A4159}"/>
-    <hyperlink ref="A71" r:id="rId70" display="https://www.pgatour.com/players/player.34363.tyrrell-hatton.html" xr:uid="{81EE9BF0-97BD-B04C-85A1-439869325861}"/>
-    <hyperlink ref="A72" r:id="rId71" display="https://www.pgatour.com/players/player.27064.jhonattan-vegas.html" xr:uid="{C7D8D3E2-1F9C-D245-9CF8-AC7EB99C9FE3}"/>
-    <hyperlink ref="A73" r:id="rId72" display="https://www.pgatour.com/players/player.34563.chesson-hadley.html" xr:uid="{2D5515E2-5A67-114F-A506-D2228CD62A95}"/>
-    <hyperlink ref="A74" r:id="rId73" display="https://www.pgatour.com/players/player.32150.michael-thompson.html" xr:uid="{8CC8AD0F-0306-154A-9B31-D76F94D953B0}"/>
-    <hyperlink ref="A75" r:id="rId74" display="https://www.pgatour.com/players/player.47347.adam-schenk.html" xr:uid="{30516970-211A-C64E-832E-ABA27DFD8CAB}"/>
-    <hyperlink ref="A76" r:id="rId75" display="https://www.pgatour.com/players/player.31560.brian-stuard.html" xr:uid="{513CC68D-CBA1-1F4A-A96D-591BEF3E17CD}"/>
-    <hyperlink ref="A77" r:id="rId76" display="https://www.pgatour.com/players/player.33948.byeong-hun-an.html" xr:uid="{B3046CE2-0B45-0949-8E87-C38EDEFD89C9}"/>
-    <hyperlink ref="A78" r:id="rId77" display="https://www.pgatour.com/players/player.56278.matthew-wolff.html" xr:uid="{606C55D7-975D-3D48-8926-345EEE6CD1B6}"/>
-    <hyperlink ref="A79" r:id="rId78" display="https://www.pgatour.com/players/player.49771.j-t--poston.html" xr:uid="{3C15925A-0370-C44F-B118-6566087066A1}"/>
-    <hyperlink ref="A80" r:id="rId79" display="https://www.pgatour.com/players/player.45486.joaquin-niemann.html" xr:uid="{31AF01A2-3FC6-5C4B-975A-DD7CECC54974}"/>
-    <hyperlink ref="A81" r:id="rId80" display="https://www.pgatour.com/players/player.27129.luke-list.html" xr:uid="{00EE624C-B1C7-2047-9AD1-6A16D64CC1F9}"/>
-    <hyperlink ref="A82" r:id="rId81" display="https://www.pgatour.com/players/player.21528.henrik-stenson.html" xr:uid="{4C4BCD09-88DD-A549-8349-FB4FFFB1BAE9}"/>
-    <hyperlink ref="A83" r:id="rId82" display="https://www.pgatour.com/players/player.47504.sam-burns.html" xr:uid="{FFEAF601-E2C7-F24A-9379-11A780D27FE5}"/>
-    <hyperlink ref="A84" r:id="rId83" display="https://www.pgatour.com/players/player.25804.bubba-watson.html" xr:uid="{F72B12CF-F0A8-3549-B83C-97C1DD03FA01}"/>
-    <hyperlink ref="A85" r:id="rId84" display="https://www.pgatour.com/players/player.51766.wyndham-clark.html" xr:uid="{10697E7B-7233-DD4B-AE3C-2CE5D1AE2C7F}"/>
-    <hyperlink ref="A86" r:id="rId85" display="https://www.pgatour.com/players/player.35891.cameron-smith.html" xr:uid="{2EC088D3-5530-904F-9D12-03B4221F7254}"/>
-    <hyperlink ref="A87" r:id="rId86" display="https://www.pgatour.com/players/player.29974.branden-grace.html" xr:uid="{3BBDA4C7-CCC3-0E41-944A-79A8C8CBB137}"/>
-    <hyperlink ref="A88" r:id="rId87" display="https://www.pgatour.com/players/player.34098.russell-henley.html" xr:uid="{1F6E9FC1-8109-CD43-A1F0-02BCCA8DCB1B}"/>
-    <hyperlink ref="A89" r:id="rId88" display="https://www.pgatour.com/players/player.39324.j-j--spaun.html" xr:uid="{FDD1B705-8119-084A-99B9-BD8E7327A1B9}"/>
-    <hyperlink ref="A90" r:id="rId89" display="https://www.pgatour.com/players/player.46402.talor-gooch.html" xr:uid="{1B84B0FE-E908-AB48-AF65-517089DE8F8B}"/>
-    <hyperlink ref="A91" r:id="rId90" display="https://www.pgatour.com/players/player.27095.nick-watney.html" xr:uid="{8FCDFD6C-164D-824A-8B28-30ACD6A3707D}"/>
-    <hyperlink ref="A92" r:id="rId91" display="https://www.pgatour.com/players/player.36699.patrick-rodgers.html" xr:uid="{CA719BD8-BE24-214F-B74D-1D4C1A45E625}"/>
-    <hyperlink ref="A93" r:id="rId92" display="https://www.pgatour.com/players/player.37189.harold-varner-iii.html" xr:uid="{97DA851A-8BB1-324A-AAB4-5ECB66C38DC0}"/>
-    <hyperlink ref="A94" r:id="rId93" display="https://www.pgatour.com/players/player.34021.bud-cauley.html" xr:uid="{3632D270-B840-CD42-9E07-7757D2E3AECC}"/>
-    <hyperlink ref="A95" r:id="rId94" display="https://www.pgatour.com/players/player.37275.sam-ryder.html" xr:uid="{7B5D6ECE-8469-7A47-B3E9-A675DBBF528E}"/>
-    <hyperlink ref="A96" r:id="rId95" display="https://www.pgatour.com/players/player.33122.russell-knox.html" xr:uid="{2BE7E443-1327-0E47-B8D7-FAA0A1FFA220}"/>
-    <hyperlink ref="A97" r:id="rId96" display="https://www.pgatour.com/players/player.27963.chris-stroud.html" xr:uid="{A085672C-77DF-C048-AED0-2CD3C97541CC}"/>
-    <hyperlink ref="A98" r:id="rId97" display="https://www.pgatour.com/players/player.32791.kyoung-hoon-lee.html" xr:uid="{0B3F6A8D-ADEA-B648-8B72-0CFC263ECAB8}"/>
-    <hyperlink ref="A99" r:id="rId98" display="https://www.pgatour.com/players/player.33419.cameron-tringale.html" xr:uid="{5BA74641-5086-664C-8E64-FBAE94B0F92F}"/>
-    <hyperlink ref="A100" r:id="rId99" display="https://www.pgatour.com/players/player.35506.mackenzie-hughes.html" xr:uid="{8A6DFA44-31A3-6640-B807-8700783EB0AC}"/>
-    <hyperlink ref="A101" r:id="rId100" display="https://www.pgatour.com/players/player.30692.scott-stallings.html" xr:uid="{D461D735-D964-314B-9032-253186BD238E}"/>
-    <hyperlink ref="A102" r:id="rId101" display="https://www.pgatour.com/players/player.29479.scott-brown.html" xr:uid="{CDA6CDE5-CE51-FE4D-83B1-652315A93886}"/>
-    <hyperlink ref="A103" r:id="rId102" display="https://www.pgatour.com/players/player.27644.brian-harman.html" xr:uid="{A97095FB-91F3-F641-9DBC-40E4E3431336}"/>
-    <hyperlink ref="A104" r:id="rId103" display="https://www.pgatour.com/players/player.33486.roger-sloan.html" xr:uid="{B1508930-767F-C64E-9C1F-81D5187AFE3B}"/>
-    <hyperlink ref="A105" r:id="rId104" display="https://www.pgatour.com/players/player.22371.aaron-baddeley.html" xr:uid="{B67CE83C-EE34-E744-88A1-27132DC66BD4}"/>
-    <hyperlink ref="A106" r:id="rId105" display="https://www.pgatour.com/players/player.34466.peter-malnati.html" xr:uid="{E997CABF-A464-C842-AABD-1528323FF9FF}"/>
-    <hyperlink ref="A107" r:id="rId106" display="https://www.pgatour.com/players/player.26300.matt-jones.html" xr:uid="{2B05BEC5-3CEA-E044-9B45-5502EFDF7310}"/>
-    <hyperlink ref="A108" r:id="rId107" display="https://www.pgatour.com/players/player.32139.danny-willett.html" xr:uid="{167219EF-D0F9-1A4F-9E8A-C838FDE96948}"/>
-    <hyperlink ref="A109" r:id="rId108" display="https://www.pgatour.com/players/player.19846.brian-gay.html" xr:uid="{4A0329F6-0341-AE4D-A07F-4E34AC8D1B5E}"/>
-    <hyperlink ref="A110" r:id="rId109" display="https://www.pgatour.com/players/player.33667.carlos-ortiz.html" xr:uid="{4B56E8D0-F3B5-0C46-814C-4D64E8C58331}"/>
-    <hyperlink ref="A111" r:id="rId110" display="https://www.pgatour.com/players/player.25493.nick-taylor.html" xr:uid="{0E875953-0005-BC48-BAA5-55519FF23B88}"/>
-    <hyperlink ref="A112" r:id="rId111" display="https://www.pgatour.com/players/player.30110.kyle-stanley.html" xr:uid="{F7323A43-C6F9-4143-8794-B6E53382E154}"/>
-    <hyperlink ref="A113" r:id="rId112" display="https://www.pgatour.com/players/player.32640.troy-merritt.html" xr:uid="{3E3B1D9B-B112-854D-B999-24DB8CD71F41}"/>
-    <hyperlink ref="A114" r:id="rId113" display="https://www.pgatour.com/players/player.19803.ryan-armour.html" xr:uid="{BBE5B9C9-2FD3-AC41-9171-4A5419FD41CA}"/>
-    <hyperlink ref="A115" r:id="rId114" display="https://www.pgatour.com/players/player.35879.kelly-kraft.html" xr:uid="{748CB978-C0DF-6E44-9728-05BBC502F890}"/>
-    <hyperlink ref="A116" r:id="rId115" display="https://www.pgatour.com/players/player.47993.denny-mccarthy.html" xr:uid="{DAECEF40-7751-564C-AC9A-9DB38401B0DA}"/>
-    <hyperlink ref="A117" r:id="rId116" display="https://www.pgatour.com/players/player.49964.aaron-wise.html" xr:uid="{61A7F96F-2079-A140-9273-6C2E3F46C6C6}"/>
-    <hyperlink ref="A118" r:id="rId117" display="https://www.pgatour.com/players/player.27895.jonas-blixt.html" xr:uid="{7E6DAFC5-519D-6A41-92B8-2EB9482A80D2}"/>
-    <hyperlink ref="A119" r:id="rId118" display="https://www.pgatour.com/players/player.29535.brice-garnett.html" xr:uid="{F289912F-BBF9-744F-81E5-D3BFDE78F0C2}"/>
-    <hyperlink ref="A120" r:id="rId119" display="https://www.pgatour.com/players/player.49960.sepp-straka.html" xr:uid="{63017A76-83C3-974D-B87A-458BBDBCFEAE}"/>
-    <hyperlink ref="A121" r:id="rId120" display="https://www.pgatour.com/players/player.24361.pat-perez.html" xr:uid="{B277A19A-4EE1-3245-A4B7-C6D0A09F03A3}"/>
-    <hyperlink ref="A122" r:id="rId121" display="https://www.pgatour.com/players/player.46435.austin-cook.html" xr:uid="{22038644-53F6-8745-960E-1AEFE51A9CE4}"/>
-    <hyperlink ref="A123" r:id="rId122" display="https://www.pgatour.com/players/player.35617.martin-trainer.html" xr:uid="{0E874759-090E-DD4E-99B4-F3139B4F45B4}"/>
-    <hyperlink ref="A124" r:id="rId123" display="https://www.pgatour.com/players/player.27936.martin-laird.html" xr:uid="{99509340-5E68-B34E-8754-25CF431400C0}"/>
-    <hyperlink ref="A125" r:id="rId124" display="https://www.pgatour.com/players/player.47128.richy-werenski.html" xr:uid="{8553B68C-5412-C342-8691-D39370CAEFBC}"/>
-    <hyperlink ref="A126" r:id="rId125" display="https://www.pgatour.com/players/player.32757.patton-kizzire.html" xr:uid="{16EF3415-D502-8641-9FEB-739A3A9E2621}"/>
-    <hyperlink ref="A127" r:id="rId126" display="https://www.pgatour.com/players/player.40026.daniel-berger.html" xr:uid="{DD4E400B-6A8E-924A-9AC7-58DDF2D3B36A}"/>
-    <hyperlink ref="A128" r:id="rId127" display="https://www.pgatour.com/players/player.33410.andrew-landry.html" xr:uid="{742871A7-DECE-EC41-97AE-08574C691BD8}"/>
-    <hyperlink ref="A129" r:id="rId128" display="https://www.pgatour.com/players/player.33418.shawn-stefani.html" xr:uid="{30B04029-0559-3045-8DAF-679FB3A0B531}"/>
-    <hyperlink ref="A130" r:id="rId129" display="https://www.pgatour.com/players/player.48822.sebastian-munoz.html" xr:uid="{48DF71B5-BAE9-7247-B5C7-C194A888A2FF}"/>
-    <hyperlink ref="A131" r:id="rId130" display="https://www.pgatour.com/players/player.35732.wes-roach.html" xr:uid="{B74513CD-9B49-7C41-A3DD-0676533F56B3}"/>
-    <hyperlink ref="A132" r:id="rId131" display="https://www.pgatour.com/players/player.25686.jason-dufner.html" xr:uid="{548E9C72-E115-B542-9065-0B9F4BB363CA}"/>
-    <hyperlink ref="A133" r:id="rId132" display="https://www.pgatour.com/players/player.29484.peter-uihlein.html" xr:uid="{1745ADC0-27D4-FB48-8D64-80796E471369}"/>
-    <hyperlink ref="A134" r:id="rId133" display="https://www.pgatour.com/players/player.27958.ryan-blaum.html" xr:uid="{7962948A-8EE9-2449-BA83-57B08193DABB}"/>
-    <hyperlink ref="A135" r:id="rId134" display="https://www.pgatour.com/players/player.31557.jim-herman.html" xr:uid="{27214ECC-17A8-AD42-A328-19863085F18D}"/>
-    <hyperlink ref="A136" r:id="rId135" display="https://www.pgatour.com/players/player.32200.roberto-castro.html" xr:uid="{741B4789-B78C-C149-A9CD-3C68764B09AF}"/>
-    <hyperlink ref="A137" r:id="rId136" display="https://www.pgatour.com/players/player.27349.alex-noren.html" xr:uid="{F8BC0C3C-3898-9E4F-A68B-5DB47938DEE8}"/>
-    <hyperlink ref="A138" r:id="rId137" display="https://www.pgatour.com/players/player.24924.bill-haas.html" xr:uid="{9C8E4561-C245-5E4A-AC42-E701B60E2F1B}"/>
-    <hyperlink ref="A139" r:id="rId138" display="https://www.pgatour.com/players/player.33449.zack-sucher.html" xr:uid="{0513F98A-2E83-5946-82BD-42B7C39847B0}"/>
-    <hyperlink ref="A140" r:id="rId139" display="https://www.pgatour.com/players/player.40009.dominic-bozzelli.html" xr:uid="{C8F45D64-677B-4141-B939-488B947E003A}"/>
-    <hyperlink ref="A141" r:id="rId140" display="https://www.pgatour.com/players/player.35461.beau-hossler.html" xr:uid="{3088FF36-5D22-7748-8FFB-D0B560F1DBD4}"/>
-    <hyperlink ref="A142" r:id="rId141" display="https://www.pgatour.com/players/player.49766.hank-lebioda.html" xr:uid="{275605FF-91EB-9C46-BC72-D116C414BD26}"/>
-    <hyperlink ref="A143" r:id="rId142" display="https://www.pgatour.com/players/player.27556.ted-potter--jr-.html" xr:uid="{70399508-72CA-D14D-9160-0A9056430C68}"/>
-    <hyperlink ref="A144" r:id="rId143" display="https://www.pgatour.com/players/player.28252.seamus-power.html" xr:uid="{D484EFBB-55FD-344D-9FBC-5A7780CC452E}"/>
-    <hyperlink ref="A145" r:id="rId144" display="https://www.pgatour.com/players/player.34431.robert-streb.html" xr:uid="{77BBA4B5-E762-C944-AD0D-061865F2E33A}"/>
-    <hyperlink ref="A146" r:id="rId145" display="https://www.pgatour.com/players/player.36799.stephan-jaeger.html" xr:uid="{8FD84877-3818-B846-A747-E2E71674BEA8}"/>
-    <hyperlink ref="A147" r:id="rId146" display="https://www.pgatour.com/players/player.29268.bronson-burgoon.html" xr:uid="{05C3BF9A-1EAF-DD4F-841F-EFFB446BBBBA}"/>
-    <hyperlink ref="A148" r:id="rId147" display="https://www.pgatour.com/players/player.34261.scott-langley.html" xr:uid="{94148671-B646-9C48-BB5F-B00358A7ADE7}"/>
-    <hyperlink ref="A149" r:id="rId148" display="https://www.pgatour.com/players/player.34099.harris-english.html" xr:uid="{96457FB8-39F1-A842-B486-4C8AB6CA8848}"/>
-    <hyperlink ref="A150" r:id="rId149" display="https://www.pgatour.com/players/player.27408.martin-kaymer.html" xr:uid="{C4C6E2A8-ACB3-7D43-8A72-FE64F6D6D6EA}"/>
-    <hyperlink ref="A151" r:id="rId150" display="https://www.pgatour.com/players/player.24024.zach-johnson.html" xr:uid="{7E56B08A-1251-4746-B627-DA2C2F55B120}"/>
-    <hyperlink ref="A152" r:id="rId151" display="https://www.pgatour.com/players/player.46601.trey-mullinax.html" xr:uid="{ADFE3682-F8EC-2C46-BDD9-118D8595A499}"/>
-    <hyperlink ref="A153" r:id="rId152" display="https://www.pgatour.com/players/player.25632.jimmy-walker.html" xr:uid="{F9F792E2-DFB8-DC48-9BBB-D80E40AD25A1}"/>
-    <hyperlink ref="A154" r:id="rId153" display="https://www.pgatour.com/players/player.24925.jonathan-byrd.html" xr:uid="{62AF8721-D6F5-804A-B3F7-080938BD4D1D}"/>
-    <hyperlink ref="A155" r:id="rId154" display="https://www.pgatour.com/players/player.49298.kramer-hickok.html" xr:uid="{17891725-D1F7-7746-82E4-EE0C3DFD4168}"/>
-    <hyperlink ref="A156" r:id="rId155" display="https://www.pgatour.com/players/player.34264.hudson-swafford.html" xr:uid="{F4F4E5EA-700C-3A49-82D8-BC4AA944F453}"/>
-    <hyperlink ref="A157" r:id="rId156" display="https://www.pgatour.com/players/player.37340.chase-wright.html" xr:uid="{B7C5E22F-FE75-444F-9AAB-691442F96E3A}"/>
-    <hyperlink ref="A158" r:id="rId157" display="https://www.pgatour.com/players/player.26951.johnson-wagner.html" xr:uid="{7468AFA6-8244-314B-BA8F-31BD3B2567C0}"/>
-    <hyperlink ref="A159" r:id="rId158" display="https://www.pgatour.com/players/player.36852.jim-knous.html" xr:uid="{E0BCD458-71A2-1745-A94E-965D631583FD}"/>
-    <hyperlink ref="A160" r:id="rId159" display="https://www.pgatour.com/players/player.23788.d-j--trahan.html" xr:uid="{857E2433-BE57-3241-B083-BC3C54C3C76B}"/>
-    <hyperlink ref="A161" r:id="rId160" display="https://www.pgatour.com/players/player.45609.tyler-duncan.html" xr:uid="{66178307-49D2-284A-86F7-34B952E589D5}"/>
-    <hyperlink ref="A162" r:id="rId161" display="https://www.pgatour.com/players/player.45157.cameron-davis.html" xr:uid="{1BC7E469-C02C-494D-817A-B3E835C34A44}"/>
-    <hyperlink ref="A163" r:id="rId162" display="https://www.pgatour.com/players/player.30946.alex-prugh.html" xr:uid="{3A7393F8-2C37-A047-9C06-CA3C5F309211}"/>
-    <hyperlink ref="A164" r:id="rId163" display="https://www.pgatour.com/players/player.46523.joey-garber.html" xr:uid="{90FD759C-FBDC-7A4A-903F-F39CC29F0CFD}"/>
-    <hyperlink ref="A165" r:id="rId164" display="https://www.pgatour.com/players/player.35376.roberto-diaz.html" xr:uid="{E04AD798-A98E-F349-A280-ACB858BEEC43}"/>
-    <hyperlink ref="A166" r:id="rId165" display="https://www.pgatour.com/players/player.49303.anders-albertson.html" xr:uid="{F181E654-6856-EB45-B9F4-D7A57CF17703}"/>
-    <hyperlink ref="A167" r:id="rId166" display="https://www.pgatour.com/players/player.40115.adam-svensson.html" xr:uid="{9249667C-FB7C-9342-ADFB-0657EBD304D4}"/>
-    <hyperlink ref="A168" r:id="rId167" display="https://www.pgatour.com/players/player.29223.sam-saunders.html" xr:uid="{7D36524F-19DC-8D40-BFB3-2CD280DB997F}"/>
-    <hyperlink ref="A169" r:id="rId168" display="https://www.pgatour.com/players/player.35421.brandon-harkins.html" xr:uid="{A7443154-80B7-EB42-9590-670DF13C56EC}"/>
-    <hyperlink ref="A170" r:id="rId169" display="https://www.pgatour.com/players/player.29518.brendan-steele.html" xr:uid="{049E0C8D-7FD7-9B43-B013-2D951406BF10}"/>
-    <hyperlink ref="A171" r:id="rId170" display="https://www.pgatour.com/players/player.26758.david-hearn.html" xr:uid="{D3B95CFA-28DD-8F49-8EFE-192A6AFE9449}"/>
-    <hyperlink ref="A172" r:id="rId171" display="https://www.pgatour.com/players/player.37380.curtis-luck.html" xr:uid="{1AED2F31-8E38-FA4B-AE95-BA46FB62682E}"/>
-    <hyperlink ref="A173" r:id="rId172" display="https://www.pgatour.com/players/player.35532.tom-hoge.html" xr:uid="{952B3871-08DF-6A4A-9D60-0AE939F6B190}"/>
-    <hyperlink ref="A174" r:id="rId173" display="https://www.pgatour.com/players/player.30191.julian-etulain.html" xr:uid="{D76A0F90-13D5-3D4D-87D0-B3A50EF75F67}"/>
-    <hyperlink ref="A175" r:id="rId174" display="https://www.pgatour.com/players/player.27330.josh-teater.html" xr:uid="{1070B0F1-FE22-0944-95C1-BEBC209EB2ED}"/>
-    <hyperlink ref="A176" r:id="rId175" display="https://www.pgatour.com/players/player.32058.jose-de-jesus-rodriguez.html" xr:uid="{EE686154-0B73-4341-AF9D-CB3B40887266}"/>
-    <hyperlink ref="A177" r:id="rId176" display="https://www.pgatour.com/players/player.20229.stewart-cink.html" xr:uid="{08067105-9A41-3F49-84DC-3895A2E77767}"/>
-    <hyperlink ref="A178" r:id="rId177" display="https://www.pgatour.com/players/player.31420.anirban-lahiri.html" xr:uid="{E38CB4EA-2EF6-EB41-B899-51B075BDE78D}"/>
-    <hyperlink ref="A179" r:id="rId178" display="https://www.pgatour.com/players/player.28679.fabian-gomez.html" xr:uid="{049896FB-86BF-374A-A752-F6741E258718}"/>
-    <hyperlink ref="A180" r:id="rId179" display="https://www.pgatour.com/players/player.46501.ollie-schniederjans.html" xr:uid="{1DB90DC0-9C87-B74C-852B-99FFCC90F975}"/>
-    <hyperlink ref="A181" r:id="rId180" display="https://www.pgatour.com/players/player.39327.ben-silverman.html" xr:uid="{04C58E33-8D90-8C4B-BE6C-DCC20DA33C58}"/>
-    <hyperlink ref="A182" r:id="rId181" display="https://www.pgatour.com/players/player.06522.ernie-els.html" xr:uid="{F925E662-13DF-9D44-B52B-AEB59FAB1DFE}"/>
-    <hyperlink ref="A183" r:id="rId182" display="https://www.pgatour.com/players/player.24781.hunter-mahan.html" xr:uid="{560A2C37-AFE9-834C-A101-6446709044D8}"/>
-    <hyperlink ref="A184" r:id="rId183" display="https://www.pgatour.com/players/player.32816.satoshi-kodaira.html" xr:uid="{1F21E75D-B4EE-5248-9137-41D1099FD239}"/>
-    <hyperlink ref="A185" r:id="rId184" display="https://www.pgatour.com/players/player.30927.brendon-todd.html" xr:uid="{95B6156F-7EBA-3F45-A68B-3C79848078B0}"/>
-    <hyperlink ref="A186" r:id="rId185" display="https://www.pgatour.com/players/player.37454.whee-kim.html" xr:uid="{D13EA653-1A53-5D4C-9113-5CABD6487E2F}"/>
-    <hyperlink ref="A187" r:id="rId186" display="https://www.pgatour.com/players/player.47856.seth-reeves.html" xr:uid="{3AB1CEDF-E809-1443-9CCD-D0ACA33E4694}"/>
-    <hyperlink ref="A188" r:id="rId187" display="https://www.pgatour.com/players/player.23983.luke-donald.html" xr:uid="{E97F9021-8E0D-064D-A17D-AFCD1FB5C404}"/>
-    <hyperlink ref="A189" r:id="rId188" display="https://www.pgatour.com/players/player.26331.charl-schwartzel.html" xr:uid="{B308D0AF-7C76-5C45-813A-A377675CF70E}"/>
-    <hyperlink ref="A190" r:id="rId189" display="https://www.pgatour.com/players/player.39954.cody-gribble.html" xr:uid="{D78CF976-AE35-BF4B-A4EE-3D47D4B6AB84}"/>
-    <hyperlink ref="A191" r:id="rId190" display="https://www.pgatour.com/players/player.32366.kevin-chappell.html" xr:uid="{EB759E9D-9A33-534C-8F96-EF8750CB03EB}"/>
-    <hyperlink ref="A192" r:id="rId191" display="https://www.pgatour.com/players/player.01706.davis-love-iii.html" xr:uid="{BE61CF0C-FB8B-F946-8F8D-390424791895}"/>
-    <hyperlink ref="A193" r:id="rId192" display="https://www.pgatour.com/players/player.47990.kyle-jones.html" xr:uid="{36E5F962-029D-174B-ACC3-352A21A55C8F}"/>
-    <hyperlink ref="A194" r:id="rId193" display="https://www.pgatour.com/players/player.30786.brady-schnell.html" xr:uid="{A28785C7-83D7-1146-A068-164CC5B363BD}"/>
-    <hyperlink ref="A195" r:id="rId194" display="https://www.pgatour.com/players/player.29222.billy-hurley-iii.html" xr:uid="{4EBF28F2-15FD-4B40-A82E-FBB5D4774980}"/>
-    <hyperlink ref="A196" r:id="rId195" display="https://www.pgatour.com/players/player.06567.vijay-singh.html" xr:uid="{8130F0A9-91C9-2A4C-8C37-A22B90A1DD8C}"/>
-    <hyperlink ref="A197" r:id="rId196" display="https://www.pgatour.com/players/player.30926.chris-kirk.html" xr:uid="{69868106-726E-7043-960B-CC6883CF623F}"/>
-    <hyperlink ref="A198" r:id="rId197" display="https://www.pgatour.com/players/player.23541.ben-crane.html" xr:uid="{D4E746D4-DCF4-A94A-9596-321578A0DFE1}"/>
-    <hyperlink ref="A199" r:id="rId198" display="https://www.pgatour.com/players/player.37278.nicholas-lindheim.html" xr:uid="{5F70F494-8DC2-8D40-965F-4BCF9E33B1BA}"/>
-    <hyperlink ref="A200" r:id="rId199" display="https://www.pgatour.com/players/player.24140.sean-o-hair.html" xr:uid="{AD32D58E-DDDC-6949-BCD7-5B9E1CF1611E}"/>
-    <hyperlink ref="A201" r:id="rId200" display="https://www.pgatour.com/players/player.23353.j-j--henry.html" xr:uid="{155A9820-DCA0-FE4A-8B6B-B6FD9A60B0A1}"/>
-    <hyperlink ref="A202" r:id="rId201" display="https://www.pgatour.com/players/player.28259.sangmoon-bae.html" xr:uid="{01FFC456-51DE-3C4F-8945-972454B092FF}"/>
-    <hyperlink ref="A203" r:id="rId202" display="https://www.pgatour.com/players/player.32876.martin-piller.html" xr:uid="{E27F58DB-7595-574A-AC5F-14C5C2CF74F4}"/>
-    <hyperlink ref="A204" r:id="rId203" display="https://www.pgatour.com/players/player.21731.freddie-jacobson.html" xr:uid="{D1B670EE-3402-D349-9906-510913A91085}"/>
-    <hyperlink ref="A205" r:id="rId204" display="https://www.pgatour.com/players/player.32448.james-hahn.html" xr:uid="{BC625549-54DF-5B4A-85FF-B73AF59D8E59}"/>
-    <hyperlink ref="A206" r:id="rId205" display="https://www.pgatour.com/players/player.50526.tom-lovelady.html" xr:uid="{824F1123-1106-A145-8F69-FF929D3F7BB2}"/>
-    <hyperlink ref="A207" r:id="rId206" display="https://www.pgatour.com/players/player.24357.k-j--choi.html" xr:uid="{F02E98D3-36EE-2743-B711-0C5B35359FAD}"/>
-    <hyperlink ref="A208" r:id="rId207" display="https://www.pgatour.com/players/player.29461.jamie-lovemark.html" xr:uid="{209225A4-B1EB-B64D-A82E-121D21DE995E}"/>
-    <hyperlink ref="A209" r:id="rId208" display="https://www.pgatour.com/players/player.20766.padraig-harrington.html" xr:uid="{43EFC705-665A-3148-BA6F-6F4960CA193F}"/>
-    <hyperlink ref="A210" r:id="rId209" display="https://www.pgatour.com/players/player.24490.george-mcneill.html" xr:uid="{8C876C2B-3A96-EF49-9D38-D34F0E2E23BE}"/>
-    <hyperlink ref="A211" r:id="rId210" display="https://www.pgatour.com/players/player.20472.alex-cejka.html" xr:uid="{79CCAFB4-D5D1-A14C-8918-F0E19622EE77}"/>
-    <hyperlink ref="A212" r:id="rId211" display="https://www.pgatour.com/players/player.34213.grayson-murray.html" xr:uid="{97B39333-101C-0C41-9E43-8CCFD73E7909}"/>
-    <hyperlink ref="A213" r:id="rId212" display="https://www.pgatour.com/players/player.28132.tyrone-van-aswegen.html" xr:uid="{D6A9F924-DEAD-1E40-BB22-D9DC023C3BD1}"/>
-    <hyperlink ref="A214" r:id="rId213" display="https://www.pgatour.com/players/player.26289.boo-weekley.html" xr:uid="{3234AEAF-5D97-384A-8D1D-FA44C74D38E4}"/>
-    <hyperlink ref="A215" r:id="rId214" display="https://www.pgatour.com/players/player.06527.steve-stricker.html" xr:uid="{B8F253CB-E99C-E249-9A88-59C5541F373B}"/>
-    <hyperlink ref="A216" r:id="rId215" display="https://www.pgatour.com/players/player.22892.jason-gore.html" xr:uid="{51F16CDE-E923-8244-9896-A61741FC73ED}"/>
-    <hyperlink ref="A217" r:id="rId216" display="https://www.pgatour.com/players/player.31416.derek-fathauer.html" xr:uid="{DCB3059C-0EF0-B749-84FB-449837FC6987}"/>
-    <hyperlink ref="A218" r:id="rId217" display="https://www.pgatour.com/players/player.34306.john-chin.html" xr:uid="{50EC4BB1-12C5-BD45-BC27-3DCEE0192898}"/>
-    <hyperlink ref="A219" r:id="rId218" display="https://www.pgatour.com/players/player.34174.john-huh.html" xr:uid="{ECAC3361-3870-264D-A1A9-DD643C9D64C8}"/>
-    <hyperlink ref="A220" r:id="rId219" display="https://www.pgatour.com/players/player.20572.rod-pampling.html" xr:uid="{FDA47DD8-AA45-E145-AF6F-0FCE033C8D6F}"/>
-    <hyperlink ref="A221" r:id="rId220" display="https://www.pgatour.com/players/player.25562.andres-romero.html" xr:uid="{74548952-030E-7140-AE31-0708D7F1E68B}"/>
-    <hyperlink ref="A222" r:id="rId221" display="https://www.pgatour.com/players/player.10387.chris-thompson.html" xr:uid="{868DAC85-9987-D044-AF78-C306ED1B9DE6}"/>
-    <hyperlink ref="A223" r:id="rId222" display="https://www.pgatour.com/players/player.02206.david-toms.html" xr:uid="{024670EE-1536-9147-B321-0A6F95499F35}"/>
-    <hyperlink ref="A224" r:id="rId223" display="https://www.pgatour.com/players/player.21407.arjun-atwal.html" xr:uid="{56251D9C-BCC0-4A4F-AB76-0CEF655CFDFB}"/>
-    <hyperlink ref="A225" r:id="rId224" display="https://www.pgatour.com/players/player.33461.morgan-hoffmann.html" xr:uid="{67E43C0D-BA20-A94E-835E-3EACB37FC496}"/>
-    <hyperlink ref="A226" r:id="rId225" display="https://www.pgatour.com/players/player.24358.robert-garrigus.html" xr:uid="{FAA06CFF-E3CD-8F4F-A10A-E1807939DCC6}"/>
-    <hyperlink ref="A227" r:id="rId226" display="https://www.pgatour.com/players/player.39975.michael-kim.html" xr:uid="{BF6ECA50-AA6A-B949-ABA9-A33322B1C84F}"/>
-    <hyperlink ref="A228" r:id="rId227" display="https://www.pgatour.com/players/player.20645.john-senden.html" xr:uid="{FC3F9459-4144-394D-B04A-77DF32BF39E4}"/>
-    <hyperlink ref="A229" r:id="rId228" display="https://www.pgatour.com/players/player.30711.colt-knost.html" xr:uid="{40803AF0-9244-5F4B-8D81-41ED2BAF9840}"/>
-    <hyperlink ref="A230" r:id="rId229" display="https://www.pgatour.com/players/player.34409.david-lingmerth.html" xr:uid="{8D89969C-F609-114D-AF4A-FF5DFF72B57D}"/>
-    <hyperlink ref="A231" r:id="rId230" display="https://www.pgatour.com/players/player.20850.daniel-chopra.html" xr:uid="{51AE3B9E-56B1-1941-988C-0780B6189BD5}"/>
-    <hyperlink ref="A232" r:id="rId231" display="https://www.pgatour.com/players/player.24663.y-e--yang.html" xr:uid="{F100B337-D20D-114D-83D4-8F8274B22B7E}"/>
-    <hyperlink ref="A233" r:id="rId232" display="https://www.pgatour.com/players/player.24449.parker-mclachlin.html" xr:uid="{FBCDB114-B78B-624D-BD70-28A1B3F6EE2A}"/>
-    <hyperlink ref="A234" r:id="rId233" display="https://www.pgatour.com/players/player.20098.stuart-appleby.html" xr:uid="{24FE7A58-A094-814D-A309-0CCFE0EF74EB}"/>
-    <hyperlink ref="A235" r:id="rId234" display="https://www.pgatour.com/players/player.25240.d-a--points.html" xr:uid="{EDFA4709-5EB6-064E-BCB4-B34CA76AB1E8}"/>
-    <hyperlink ref="A236" r:id="rId235" display="https://www.pgatour.com/players/player.11123.chris-couch.html" xr:uid="{9E6E70BD-3026-6F44-91C6-DFFB0BBCD286}"/>
-    <hyperlink ref="A237" r:id="rId236" display="https://www.pgatour.com/players/player.25720.chad-collins.html" xr:uid="{0C51DA1B-8474-0C43-951B-A465F91E443E}"/>
-    <hyperlink ref="A238" r:id="rId237" display="https://www.pgatour.com/players/player.12510.chad-campbell.html" xr:uid="{545921FA-7F9C-AB40-BA14-44B17BE78848}"/>
-    <hyperlink ref="A239" r:id="rId238" display="https://www.pgatour.com/players/player.12782.tim-herron.html" xr:uid="{67ACAF1E-3B7A-5840-9F6D-DDCCDEE341D2}"/>
-    <hyperlink ref="A240" r:id="rId239" display="https://www.pgatour.com/players/player.01226.fred-couples.html" xr:uid="{853CE7AB-76D1-A14A-856D-28298C1F30AA}"/>
-    <hyperlink ref="A241" r:id="rId240" display="https://www.pgatour.com/players/player.32334.charlie-beljan.html" xr:uid="{D8D6E5DC-E659-C145-9FDE-7912302CB6FB}"/>
-    <hyperlink ref="A242" r:id="rId241" display="https://www.pgatour.com/players/player.22378.trevor-immelman.html" xr:uid="{115B72F5-4094-514A-BEA5-FDB5A4FFD0FA}"/>
-    <hyperlink ref="A243" r:id="rId242" display="https://www.pgatour.com/players/player.30750.tommy-gainey.html" xr:uid="{4EAAAC24-9849-A14B-B4C3-32375923A61E}"/>
-    <hyperlink ref="A244" r:id="rId243" display="https://www.pgatour.com/players/player.24846.ricky-barnes.html" xr:uid="{25DAE03A-09B3-E641-A563-1BDFC9F86289}"/>
-    <hyperlink ref="A245" r:id="rId244" display="https://www.pgatour.com/players/player.21753.brian-davis.html" xr:uid="{BFF4FA54-D5BE-1545-8C3F-222FCEF3B170}"/>
-    <hyperlink ref="A246" r:id="rId245" display="https://www.pgatour.com/players/player.27933.john-merrick.html" xr:uid="{98DAE846-6396-DF41-97B2-2E40E925624B}"/>
-    <hyperlink ref="A247" r:id="rId246" display="https://www.pgatour.com/players/player.22913.john-rollins.html" xr:uid="{EEE30012-2903-BC45-B808-0A9307C6C394}"/>
-    <hyperlink ref="A248" r:id="rId247" display="https://www.pgatour.com/players/player.10423.mike-weir.html" xr:uid="{95734D57-375C-2044-A107-B538CD5B8131}"/>
-    <hyperlink ref="A249" r:id="rId248" display="https://www.pgatour.com/players/player.01666.bernhard-langer.html" xr:uid="{EFE30783-179D-2C4C-AB17-4B4FA07B5DF0}"/>
-    <hyperlink ref="A250" r:id="rId249" display="https://www.pgatour.com/players/player.10885.robert-allenby.html" xr:uid="{4F8AC48C-9A6C-1D4F-B46C-60ACECC40FB0}"/>
-    <hyperlink ref="A251" r:id="rId250" display="https://www.pgatour.com/players/player.01677.tom-lehman.html" xr:uid="{28C585BE-79D7-C843-9D7D-25FA601F2CA4}"/>
-    <hyperlink ref="A252" r:id="rId251" display="https://www.pgatour.com/players/player.37273.derek-ernst.html" xr:uid="{64D3CE89-92BC-D84F-AB31-B9CA18EDEAF1}"/>
-    <hyperlink ref="A253" r:id="rId252" display="https://www.pgatour.com/players/player.46550.brandon-hagy.html" xr:uid="{A3EC22EE-6B42-D24D-85A1-30CA4AEC7DEF}"/>
-    <hyperlink ref="A254" r:id="rId253" display="https://www.pgatour.com/players/player.20160.charlie-wi.html" xr:uid="{1BB5E480-C952-744C-B333-7F44DFD4D3C0}"/>
-    <hyperlink ref="A255" r:id="rId254" display="https://www.pgatour.com/players/player.46440.smylie-kaufman.html" xr:uid="{2E74937A-9B33-D24D-809B-7CFAE8BDAB43}"/>
-    <hyperlink ref="A256" r:id="rId255" display="https://www.pgatour.com/players/player.20104.ken-duke.html" xr:uid="{E766E77E-2855-3449-B07E-969639BF42D8}"/>
-    <hyperlink ref="A257" r:id="rId256" display="https://www.pgatour.com/players/player.10213.dicky-pride.html" xr:uid="{88A410EF-FC77-734C-AD2A-1791E51570BA}"/>
-    <hyperlink ref="A258" r:id="rId257" display="https://www.pgatour.com/players/player.23614.rich-beem.html" xr:uid="{693F2822-90FD-DD4B-A61C-B6A16D405BD7}"/>
-    <hyperlink ref="A259" r:id="rId258" display="https://www.pgatour.com/players/player.23638.brendon-de-jonge.html" xr:uid="{02909326-038E-E84F-AF40-A9888F0739A3}"/>
-    <hyperlink ref="A260" r:id="rId259" display="https://www.pgatour.com/players/player.24507.jason-bohn.html" xr:uid="{ACE34B9C-5779-824C-9EB6-EFC17C4B92B5}"/>
-    <hyperlink ref="A261" r:id="rId260" display="https://www.pgatour.com/players/player.20094.jonathan-kaye.html" xr:uid="{7941DDAD-9A72-6140-8FB5-DF8EF5C37A84}"/>
-    <hyperlink ref="A262" r:id="rId261" display="https://www.pgatour.com/players/player.08385.omar-uresti.html" xr:uid="{2EB77890-FCFB-B04F-9CA3-FC734C5C3EF7}"/>
-    <hyperlink ref="A263" r:id="rId262" display="https://www.pgatour.com/players/player.22293.heath-slocum.html" xr:uid="{7BE18697-37FA-AA42-A64B-C75E868A4A9C}"/>
-    <hyperlink ref="A264" r:id="rId263" display="https://www.pgatour.com/players/player.24912.will-mackenzie.html" xr:uid="{33ABCB08-4E7A-EC47-B721-336AD1F6FCF6}"/>
+    <hyperlink ref="B2" r:id="rId1" display="https://www.pgatour.com/players/player.36689.brooks-koepka.html" xr:uid="{1399459C-416F-5B49-B207-6ABBE54EC626}"/>
+    <hyperlink ref="B3" r:id="rId2" display="https://www.pgatour.com/players/player.23108.matt-kuchar.html" xr:uid="{D9360241-A8FA-E842-A648-D5F510BE4205}"/>
+    <hyperlink ref="B4" r:id="rId3" display="https://www.pgatour.com/players/player.28237.rory-mcilroy.html" xr:uid="{3F219576-7C68-524F-8274-AEE0CE0AF1FB}"/>
+    <hyperlink ref="B5" r:id="rId4" display="https://www.pgatour.com/players/player.48081.xander-schauffele.html" xr:uid="{857590CA-AE1D-4B43-A431-F5DB088BFB24}"/>
+    <hyperlink ref="B6" r:id="rId5" display="https://www.pgatour.com/players/player.31323.gary-woodland.html" xr:uid="{76F22FC0-BCD7-EE43-8A86-A9B5D53BE391}"/>
+    <hyperlink ref="B7" r:id="rId6" display="https://www.pgatour.com/players/player.35450.patrick-cantlay.html" xr:uid="{0326ADDB-04C6-A545-975C-7C32649F8CA4}"/>
+    <hyperlink ref="B8" r:id="rId7" display="https://www.pgatour.com/players/player.30925.dustin-johnson.html" xr:uid="{1AEBBEEE-84DC-9C4F-84C6-313A0FE86F7A}"/>
+    <hyperlink ref="B9" r:id="rId8" display="https://www.pgatour.com/players/player.25364.paul-casey.html" xr:uid="{06D7D9AB-8F8E-4A48-8E4D-384B87EE2390}"/>
+    <hyperlink ref="B10" r:id="rId9" display="https://www.pgatour.com/players/player.32102.rickie-fowler.html" xr:uid="{59C94777-FEA7-A24B-802D-0B035645633D}"/>
+    <hyperlink ref="B11" r:id="rId10" display="https://www.pgatour.com/players/player.46970.jon-rahm.html" xr:uid="{3BDFA669-949D-4344-9F04-57DB6D31CA1E}"/>
+    <hyperlink ref="B12" r:id="rId11" display="https://www.pgatour.com/players/player.22405.justin-rose.html" xr:uid="{CDDFF6ED-EC8A-F54D-8D40-BD06C07DA118}"/>
+    <hyperlink ref="B13" r:id="rId12" display="https://www.pgatour.com/players/player.26476.chez-reavie.html" xr:uid="{4E8BE882-704E-5F4C-9332-4202B479162D}"/>
+    <hyperlink ref="B14" r:id="rId13" display="https://www.pgatour.com/players/player.29725.tony-finau.html" xr:uid="{9400D1E6-5EF7-CB49-AF5D-3A02870DDD29}"/>
+    <hyperlink ref="B15" r:id="rId14" display="https://www.pgatour.com/players/player.21961.charles-howell-iii.html" xr:uid="{2173B152-47BA-4649-86C6-CAB7C789DA92}"/>
+    <hyperlink ref="B16" r:id="rId15" display="https://www.pgatour.com/players/player.26851.marc-leishman.html" xr:uid="{CF98B909-50E1-9242-9EB1-D375403505E1}"/>
+    <hyperlink ref="B17" r:id="rId16" display="https://www.pgatour.com/players/player.47959.bryson-dechambeau.html" xr:uid="{64829CA7-0982-A14B-94F7-73ECFCDBA07B}"/>
+    <hyperlink ref="B18" r:id="rId17" display="https://www.pgatour.com/players/player.33448.justin-thomas.html" xr:uid="{79D65E58-9927-2E40-B0CB-97B7B21FB559}"/>
+    <hyperlink ref="B19" r:id="rId18" display="https://www.pgatour.com/players/player.33204.shane-lowry.html" xr:uid="{6F1AF1F4-6F37-6F40-868F-476713D841BB}"/>
+    <hyperlink ref="B20" r:id="rId19" display="https://www.pgatour.com/players/player.24502.adam-scott.html" xr:uid="{EFDF088D-4D21-D44E-93E4-C3D508A65078}"/>
+    <hyperlink ref="B21" r:id="rId20" display="https://www.pgatour.com/players/player.30911.tommy-fleetwood.html" xr:uid="{3C9FA0E8-DDE8-2A49-8B48-5F7CB5685DE3}"/>
+    <hyperlink ref="B22" r:id="rId21" display="https://www.pgatour.com/players/player.29478.kevin-kisner.html" xr:uid="{0D1B471F-EC79-3B49-8C8A-4EA5EBE77171}"/>
+    <hyperlink ref="B23" r:id="rId22" display="https://www.pgatour.com/players/player.25198.francesco-molinari.html" xr:uid="{A0D1EFA8-2BCC-7643-9BAE-6752427B7A9E}"/>
+    <hyperlink ref="B24" r:id="rId23" display="https://www.pgatour.com/players/player.23320.ryan-palmer.html" xr:uid="{58EEC010-C141-9649-89D9-9DC3E888721C}"/>
+    <hyperlink ref="B25" r:id="rId24" display="https://www.pgatour.com/players/player.39971.sungjae-im.html" xr:uid="{989595AB-9697-7448-9D65-0BA488DE10BE}"/>
+    <hyperlink ref="B26" r:id="rId25" display="https://www.pgatour.com/players/player.25818.scott-piercy.html" xr:uid="{ECA0967E-C38D-464B-90D5-36CC631E8CFF}"/>
+    <hyperlink ref="B27" r:id="rId26" display="https://www.pgatour.com/players/player.29221.webb-simpson.html" xr:uid="{73A46769-0F03-A549-A78E-09448E42783D}"/>
+    <hyperlink ref="B28" r:id="rId27" display="https://www.pgatour.com/players/player.08793.tiger-woods.html" xr:uid="{8B724CB7-0B6C-F546-8955-393EB17FDA1A}"/>
+    <hyperlink ref="B29" r:id="rId28" display="https://www.pgatour.com/players/player.27974.sung-kang.html" xr:uid="{EF0A244F-92AB-0E4E-BFA6-3CADD06F9873}"/>
+    <hyperlink ref="B30" r:id="rId29" display="https://www.pgatour.com/players/player.32839.hideki-matsuyama.html" xr:uid="{959BF2BD-C7FA-1C44-B650-7891BA56D63F}"/>
+    <hyperlink ref="B31" r:id="rId30" display="https://www.pgatour.com/players/player.25900.lucas-glover.html" xr:uid="{6A4A734B-DD06-2B41-B89C-4EF5096C64EC}"/>
+    <hyperlink ref="B32" r:id="rId31" display="https://www.pgatour.com/players/player.39997.corey-conners.html" xr:uid="{1FE3B402-09F3-414A-9610-360B7F98DEFC}"/>
+    <hyperlink ref="B33" r:id="rId32" display="https://www.pgatour.com/players/player.01810.phil-mickelson.html" xr:uid="{5FCA1A65-F3C7-7344-B486-C48054C7F963}"/>
+    <hyperlink ref="B34" r:id="rId33" display="https://www.pgatour.com/players/player.27649.brandt-snedeker.html" xr:uid="{5966E574-D785-BF4B-BF79-CD29CE3792E1}"/>
+    <hyperlink ref="B35" r:id="rId34" display="https://www.pgatour.com/players/player.29908.c-t--pan.html" xr:uid="{DA277624-92DF-2940-890B-E301A693B8AF}"/>
+    <hyperlink ref="B36" r:id="rId35" display="https://www.pgatour.com/players/player.39546.keith-mitchell.html" xr:uid="{E08FEB6D-2824-1B4D-8EE1-7E0CD908C3E2}"/>
+    <hyperlink ref="B37" r:id="rId36" display="https://www.pgatour.com/players/player.32333.kevin-tway.html" xr:uid="{FF0748B3-B51F-E244-9788-B520C98238C5}"/>
+    <hyperlink ref="B38" r:id="rId37" display="https://www.pgatour.com/players/player.28089.jason-day.html" xr:uid="{3272DAD3-90CF-BF42-A38B-8579655588B0}"/>
+    <hyperlink ref="B39" r:id="rId38" display="https://www.pgatour.com/players/player.10809.jim-furyk.html" xr:uid="{26620EC3-275C-B047-8275-D0A19CE079A4}"/>
+    <hyperlink ref="B40" r:id="rId39" display="https://www.pgatour.com/players/player.34256.andrew-putnam.html" xr:uid="{CCE94A8B-6593-2149-9EDE-6C30C5AFCA19}"/>
+    <hyperlink ref="B41" r:id="rId40" display="https://www.pgatour.com/players/player.33399.adam-hadwin.html" xr:uid="{A22DCD29-3519-9642-B728-93ABC9BED5A2}"/>
+    <hyperlink ref="B42" r:id="rId41" display="https://www.pgatour.com/players/player.23621.rory-sabbatini.html" xr:uid="{AF12615F-227F-234A-A4FE-764CA195746B}"/>
+    <hyperlink ref="B43" r:id="rId42" display="https://www.pgatour.com/players/player.27141.j-b--holmes.html" xr:uid="{7C7CC970-EEA0-C84C-BEC1-172F199EF0B1}"/>
+    <hyperlink ref="B44" r:id="rId43" display="https://www.pgatour.com/players/player.25396.kevin-na.html" xr:uid="{16CFCCE4-F522-AB4A-B03D-F6A195D8BD6A}"/>
+    <hyperlink ref="B45" r:id="rId44" display="https://www.pgatour.com/players/player.28775.nate-lashley.html" xr:uid="{FDE4D4EB-3878-B54B-B525-B4E3F2770483}"/>
+    <hyperlink ref="B46" r:id="rId45" display="https://www.pgatour.com/players/player.30944.jason-kokrak.html" xr:uid="{6D60D04E-B61D-1748-A868-B3BE29941D31}"/>
+    <hyperlink ref="B47" r:id="rId46" display="https://www.pgatour.com/players/player.39977.max-homa.html" xr:uid="{7499E4F1-5243-814D-91B0-7EDFB03FF80E}"/>
+    <hyperlink ref="B48" r:id="rId47" display="https://www.pgatour.com/players/player.29970.dylan-frittelli.html" xr:uid="{7729E651-0211-FC44-9822-D39BB1276F36}"/>
+    <hyperlink ref="B49" r:id="rId48" display="https://www.pgatour.com/players/player.25572.graeme-mcdowell.html" xr:uid="{5CF05B6A-2DBB-204A-B3EA-FEED666E9930}"/>
+    <hyperlink ref="B50" r:id="rId49" display="https://www.pgatour.com/players/player.37455.si-woo-kim.html" xr:uid="{A578E45A-47A9-BE46-A25A-3E225BF57295}"/>
+    <hyperlink ref="B51" r:id="rId50" display="https://www.pgatour.com/players/player.34076.joel-dahmen.html" xr:uid="{51DA22AA-F941-F643-9E44-28AA46713F8B}"/>
+    <hyperlink ref="B52" r:id="rId51" display="https://www.pgatour.com/players/player.26329.louis-oosthuizen.html" xr:uid="{27FC8ACA-DF55-B14C-BF08-FDB3A57EEA85}"/>
+    <hyperlink ref="B53" r:id="rId52" display="https://www.pgatour.com/players/player.33141.keegan-bradley.html" xr:uid="{1739FF41-0616-3644-89FB-D697749D2C15}"/>
+    <hyperlink ref="B54" r:id="rId53" display="https://www.pgatour.com/players/player.26596.ryan-moore.html" xr:uid="{228B209F-2CDC-6347-9251-1886018E1152}"/>
+    <hyperlink ref="B55" r:id="rId54" display="https://www.pgatour.com/players/player.34360.patrick-reed.html" xr:uid="{DF3F2280-9739-2B48-B2DF-9C616E56610F}"/>
+    <hyperlink ref="B56" r:id="rId55" display="https://www.pgatour.com/players/player.35449.adam-long.html" xr:uid="{7D1C7A76-C18B-6840-BF64-8A09692CAB71}"/>
+    <hyperlink ref="B57" r:id="rId56" display="https://www.pgatour.com/players/player.29420.billy-horschel.html" xr:uid="{EC67D7AF-C457-E64C-9B4B-A3A81B1BCF5D}"/>
+    <hyperlink ref="B58" r:id="rId57" display="https://www.pgatour.com/players/player.31646.emiliano-grillo.html" xr:uid="{4BAB792B-0E98-924A-9DFE-75E14B5969CE}"/>
+    <hyperlink ref="B59" r:id="rId58" display="https://www.pgatour.com/players/player.52372.cameron-champ.html" xr:uid="{3D3B2664-B7A9-F04E-899F-1AAA160F93AE}"/>
+    <hyperlink ref="B60" r:id="rId59" display="https://www.pgatour.com/players/player.26499.rafa-cabrera-bello.html" xr:uid="{60C416D0-095F-D044-AC20-BE5F9BC3906D}"/>
+    <hyperlink ref="B61" r:id="rId60" display="https://www.pgatour.com/players/player.23325.vaughn-taylor.html" xr:uid="{08C135D5-C977-1743-B345-3B3B5ECE5EFE}"/>
+    <hyperlink ref="B62" r:id="rId61" display="https://www.pgatour.com/players/player.29926.danny-lee.html" xr:uid="{89DF151C-6B1C-A54D-B743-EB400BC2B3BA}"/>
+    <hyperlink ref="B63" r:id="rId62" display="https://www.pgatour.com/players/player.45526.abraham-ancer.html" xr:uid="{257AF266-6F85-D548-B174-43F69884F2AE}"/>
+    <hyperlink ref="B64" r:id="rId63" display="https://www.pgatour.com/players/player.21209.sergio-garcia.html" xr:uid="{15CBA1DB-F101-5C45-9D35-DFC75356A700}"/>
+    <hyperlink ref="B65" r:id="rId64" display="https://www.pgatour.com/players/player.27214.kevin-streelman.html" xr:uid="{4FC30AE2-3982-D54E-BD37-A0DE7A74EA92}"/>
+    <hyperlink ref="B66" r:id="rId65" display="https://www.pgatour.com/players/player.24138.ian-poulter.html" xr:uid="{BAC76A7F-3FE9-6A4E-B97F-C7A2D1E60F2D}"/>
+    <hyperlink ref="B67" r:id="rId66" display="https://www.pgatour.com/players/player.12716.charley-hoffman.html" xr:uid="{6AF2220B-7AA3-1B4F-B3DD-180634185514}"/>
+    <hyperlink ref="B68" r:id="rId67" display="https://www.pgatour.com/players/player.30978.kiradech-aphibarnrat.html" xr:uid="{5F6BC08F-A048-CC40-88BE-B278FA906F56}"/>
+    <hyperlink ref="B69" r:id="rId68" display="https://www.pgatour.com/players/player.28307.matt-every.html" xr:uid="{2AB83BE9-E776-6340-B2CA-BBA408030CB0}"/>
+    <hyperlink ref="B70" r:id="rId69" display="https://www.pgatour.com/players/player.34046.jordan-spieth.html" xr:uid="{C40CA5F6-5AF3-074C-8FFB-03216794FA0B}"/>
+    <hyperlink ref="B71" r:id="rId70" display="https://www.pgatour.com/players/player.34363.tyrrell-hatton.html" xr:uid="{628FA638-A8F9-F944-AC51-A1705ACA353D}"/>
+    <hyperlink ref="B72" r:id="rId71" display="https://www.pgatour.com/players/player.27064.jhonattan-vegas.html" xr:uid="{BD081C54-C323-084D-A15F-76878A7AB091}"/>
+    <hyperlink ref="B73" r:id="rId72" display="https://www.pgatour.com/players/player.34563.chesson-hadley.html" xr:uid="{7AB46FE7-3B75-E94F-836B-C127F566F4F2}"/>
+    <hyperlink ref="B74" r:id="rId73" display="https://www.pgatour.com/players/player.32150.michael-thompson.html" xr:uid="{FCFF8E1D-161C-064D-B73A-0F7CD6587F7B}"/>
+    <hyperlink ref="B75" r:id="rId74" display="https://www.pgatour.com/players/player.47347.adam-schenk.html" xr:uid="{BD42484B-BAFB-7344-B9A1-55469664A1C0}"/>
+    <hyperlink ref="B76" r:id="rId75" display="https://www.pgatour.com/players/player.31560.brian-stuard.html" xr:uid="{70528B58-8A6E-5946-B893-213B0D5E220B}"/>
+    <hyperlink ref="B77" r:id="rId76" display="https://www.pgatour.com/players/player.33948.byeong-hun-an.html" xr:uid="{251DFE10-CCEC-5045-AED7-DEE89324BBA8}"/>
+    <hyperlink ref="B78" r:id="rId77" display="https://www.pgatour.com/players/player.56278.matthew-wolff.html" xr:uid="{367B5CE0-4058-2647-92A3-2C7587D397D0}"/>
+    <hyperlink ref="B79" r:id="rId78" display="https://www.pgatour.com/players/player.49771.j-t--poston.html" xr:uid="{AF86FD55-55BD-954F-B6C8-52EE6210559D}"/>
+    <hyperlink ref="B80" r:id="rId79" display="https://www.pgatour.com/players/player.45486.joaquin-niemann.html" xr:uid="{7C90930A-7348-3A4F-BD4A-BAFEC0774DF8}"/>
+    <hyperlink ref="B81" r:id="rId80" display="https://www.pgatour.com/players/player.27129.luke-list.html" xr:uid="{0ED82D6C-58FC-C245-8E2F-F5812DF45DB3}"/>
+    <hyperlink ref="B82" r:id="rId81" display="https://www.pgatour.com/players/player.21528.henrik-stenson.html" xr:uid="{601AC24C-1AE7-B34B-89A0-5A3C1C09B183}"/>
+    <hyperlink ref="B83" r:id="rId82" display="https://www.pgatour.com/players/player.47504.sam-burns.html" xr:uid="{73CD6E43-0338-064F-81F2-390669AB4643}"/>
+    <hyperlink ref="B84" r:id="rId83" display="https://www.pgatour.com/players/player.25804.bubba-watson.html" xr:uid="{3C499D4F-A7BD-BD40-9AC6-2EED9120DC78}"/>
+    <hyperlink ref="B85" r:id="rId84" display="https://www.pgatour.com/players/player.51766.wyndham-clark.html" xr:uid="{E056DB61-D289-D441-BDEF-8CF117F825E5}"/>
+    <hyperlink ref="B86" r:id="rId85" display="https://www.pgatour.com/players/player.35891.cameron-smith.html" xr:uid="{EF4EA4F2-2175-A14F-ABDE-9CBA5C4C04D9}"/>
+    <hyperlink ref="B87" r:id="rId86" display="https://www.pgatour.com/players/player.29974.branden-grace.html" xr:uid="{623DDC58-9799-4949-98D3-099E44BCC354}"/>
+    <hyperlink ref="B88" r:id="rId87" display="https://www.pgatour.com/players/player.34098.russell-henley.html" xr:uid="{0368D740-BAC0-2949-8D5E-C4360F4DE5CA}"/>
+    <hyperlink ref="B89" r:id="rId88" display="https://www.pgatour.com/players/player.39324.j-j--spaun.html" xr:uid="{210BAE1A-E3F9-B441-A686-A66C9FA5FD80}"/>
+    <hyperlink ref="B90" r:id="rId89" display="https://www.pgatour.com/players/player.46402.talor-gooch.html" xr:uid="{7093D9AA-824C-644C-8C9D-A376658F1693}"/>
+    <hyperlink ref="B91" r:id="rId90" display="https://www.pgatour.com/players/player.27095.nick-watney.html" xr:uid="{FDA5150A-7A96-B546-8569-FDD8B8B3792C}"/>
+    <hyperlink ref="B92" r:id="rId91" display="https://www.pgatour.com/players/player.36699.patrick-rodgers.html" xr:uid="{52E7F59A-8243-744D-8BA1-011BC4773762}"/>
+    <hyperlink ref="B93" r:id="rId92" display="https://www.pgatour.com/players/player.37189.harold-varner-iii.html" xr:uid="{F28C0B08-397B-F244-99EA-5D80AC41BC0D}"/>
+    <hyperlink ref="B94" r:id="rId93" display="https://www.pgatour.com/players/player.34021.bud-cauley.html" xr:uid="{2514CBD9-4BE7-6744-B8FA-06A010800BE3}"/>
+    <hyperlink ref="B95" r:id="rId94" display="https://www.pgatour.com/players/player.37275.sam-ryder.html" xr:uid="{57F5855D-B6FB-594B-8A09-32DAA99E6EF0}"/>
+    <hyperlink ref="B96" r:id="rId95" display="https://www.pgatour.com/players/player.33122.russell-knox.html" xr:uid="{E081138E-A128-3E46-9DEF-D0669D14B9C0}"/>
+    <hyperlink ref="B97" r:id="rId96" display="https://www.pgatour.com/players/player.27963.chris-stroud.html" xr:uid="{59FE9205-9EEC-0745-8F0E-18F456957E4F}"/>
+    <hyperlink ref="B98" r:id="rId97" display="https://www.pgatour.com/players/player.32791.kyoung-hoon-lee.html" xr:uid="{4C38B174-9EB7-DA41-A84F-A85DD1BC5CCD}"/>
+    <hyperlink ref="B99" r:id="rId98" display="https://www.pgatour.com/players/player.33419.cameron-tringale.html" xr:uid="{13A91D0E-EB8E-4842-A95A-DD14602E0946}"/>
+    <hyperlink ref="B100" r:id="rId99" display="https://www.pgatour.com/players/player.35506.mackenzie-hughes.html" xr:uid="{4E1BD2B4-62AD-BB44-B0D9-202F41F1E958}"/>
+    <hyperlink ref="B101" r:id="rId100" display="https://www.pgatour.com/players/player.30692.scott-stallings.html" xr:uid="{7022BD63-DC38-1E46-B489-C67AB4CF62BB}"/>
+    <hyperlink ref="B102" r:id="rId101" display="https://www.pgatour.com/players/player.29479.scott-brown.html" xr:uid="{73F8BE47-F176-3A42-93AE-01639C42C2C7}"/>
+    <hyperlink ref="B103" r:id="rId102" display="https://www.pgatour.com/players/player.27644.brian-harman.html" xr:uid="{F8C8AB18-326E-BD4C-A056-7BEF9AF22B95}"/>
+    <hyperlink ref="B104" r:id="rId103" display="https://www.pgatour.com/players/player.33486.roger-sloan.html" xr:uid="{AEF9C8F6-9471-5044-854D-CDD29EE9B895}"/>
+    <hyperlink ref="B105" r:id="rId104" display="https://www.pgatour.com/players/player.22371.aaron-baddeley.html" xr:uid="{33D12B79-C371-4141-8D18-3DBEDF53015E}"/>
+    <hyperlink ref="B106" r:id="rId105" display="https://www.pgatour.com/players/player.34466.peter-malnati.html" xr:uid="{B97F0940-53B1-A043-B5E3-7FD508B7D153}"/>
+    <hyperlink ref="B107" r:id="rId106" display="https://www.pgatour.com/players/player.26300.matt-jones.html" xr:uid="{FBF1307C-EF73-414F-AB7F-3F9A2A0693FB}"/>
+    <hyperlink ref="B108" r:id="rId107" display="https://www.pgatour.com/players/player.32139.danny-willett.html" xr:uid="{CFB2E794-8D13-3942-80F1-C28B401F242D}"/>
+    <hyperlink ref="B109" r:id="rId108" display="https://www.pgatour.com/players/player.19846.brian-gay.html" xr:uid="{0E200C8A-D235-A84D-BDC6-2D9E8E4BB464}"/>
+    <hyperlink ref="B110" r:id="rId109" display="https://www.pgatour.com/players/player.33667.carlos-ortiz.html" xr:uid="{BBEB36AA-C1EE-1D4E-8C97-C9800EBA2B8A}"/>
+    <hyperlink ref="B111" r:id="rId110" display="https://www.pgatour.com/players/player.25493.nick-taylor.html" xr:uid="{1299967F-F823-EA4C-A698-6B95B062C6E8}"/>
+    <hyperlink ref="B112" r:id="rId111" display="https://www.pgatour.com/players/player.30110.kyle-stanley.html" xr:uid="{B8AEDB23-1CBB-244A-BF7D-4A1801D82F84}"/>
+    <hyperlink ref="B113" r:id="rId112" display="https://www.pgatour.com/players/player.32640.troy-merritt.html" xr:uid="{E9A4829C-CB45-1943-A6CD-2B258CA65D79}"/>
+    <hyperlink ref="B114" r:id="rId113" display="https://www.pgatour.com/players/player.19803.ryan-armour.html" xr:uid="{1C99ED86-68FA-0747-AEC7-DB3A4801BCD9}"/>
+    <hyperlink ref="B115" r:id="rId114" display="https://www.pgatour.com/players/player.35879.kelly-kraft.html" xr:uid="{09E07618-7F42-2849-B7E6-299E2DE7F897}"/>
+    <hyperlink ref="B116" r:id="rId115" display="https://www.pgatour.com/players/player.47993.denny-mccarthy.html" xr:uid="{8739A4BA-E6CE-6E4C-AD44-F7CF52A93314}"/>
+    <hyperlink ref="B117" r:id="rId116" display="https://www.pgatour.com/players/player.49964.aaron-wise.html" xr:uid="{04D25FA6-A0CE-4B40-B467-50EC3199E363}"/>
+    <hyperlink ref="B118" r:id="rId117" display="https://www.pgatour.com/players/player.27895.jonas-blixt.html" xr:uid="{E46AFD30-1CB0-4F40-A1E5-DE2190BC237E}"/>
+    <hyperlink ref="B119" r:id="rId118" display="https://www.pgatour.com/players/player.29535.brice-garnett.html" xr:uid="{A933EA57-EBAF-1E44-A2A7-0BFAC24C5AFC}"/>
+    <hyperlink ref="B120" r:id="rId119" display="https://www.pgatour.com/players/player.49960.sepp-straka.html" xr:uid="{9B91B24F-18F7-7E4D-8172-5FC1734390B7}"/>
+    <hyperlink ref="B121" r:id="rId120" display="https://www.pgatour.com/players/player.24361.pat-perez.html" xr:uid="{93668318-BA29-3F4F-A1BF-0ABE903D93CC}"/>
+    <hyperlink ref="B122" r:id="rId121" display="https://www.pgatour.com/players/player.46435.austin-cook.html" xr:uid="{0CAF45DC-4BD2-344E-91A6-12578E2CF72F}"/>
+    <hyperlink ref="B123" r:id="rId122" display="https://www.pgatour.com/players/player.35617.martin-trainer.html" xr:uid="{5A7423EB-BC05-FF46-A2A6-A553FB1E4495}"/>
+    <hyperlink ref="B124" r:id="rId123" display="https://www.pgatour.com/players/player.27936.martin-laird.html" xr:uid="{47137E15-E20B-7747-B23C-EA4A360B91EF}"/>
+    <hyperlink ref="B125" r:id="rId124" display="https://www.pgatour.com/players/player.47128.richy-werenski.html" xr:uid="{7470066E-4D9D-474C-824D-AF78ACFADFC5}"/>
+    <hyperlink ref="B126" r:id="rId125" display="https://www.pgatour.com/players/player.32757.patton-kizzire.html" xr:uid="{98940965-CC05-CA40-856E-EB1217C24C70}"/>
+    <hyperlink ref="B127" r:id="rId126" display="https://www.pgatour.com/players/player.40026.daniel-berger.html" xr:uid="{8F54FF2F-ADD4-F64A-8261-98B29FCF47A3}"/>
+    <hyperlink ref="B128" r:id="rId127" display="https://www.pgatour.com/players/player.33410.andrew-landry.html" xr:uid="{C8DC0246-F5B7-1D41-A768-D25BD7712BA1}"/>
+    <hyperlink ref="B129" r:id="rId128" display="https://www.pgatour.com/players/player.33418.shawn-stefani.html" xr:uid="{900458AF-D9D1-2C48-9E9D-9CDC1772DF88}"/>
+    <hyperlink ref="B130" r:id="rId129" display="https://www.pgatour.com/players/player.48822.sebastian-munoz.html" xr:uid="{A720F16C-4FF5-124E-9F2C-E89B17A3A116}"/>
+    <hyperlink ref="B131" r:id="rId130" display="https://www.pgatour.com/players/player.35732.wes-roach.html" xr:uid="{F7A8F870-7B56-EA44-9EB4-DB5C39F80E68}"/>
+    <hyperlink ref="B132" r:id="rId131" display="https://www.pgatour.com/players/player.25686.jason-dufner.html" xr:uid="{C9E4D33C-B521-4B44-B913-3A311CD26B3B}"/>
+    <hyperlink ref="B133" r:id="rId132" display="https://www.pgatour.com/players/player.29484.peter-uihlein.html" xr:uid="{F69DDB9B-08D5-1444-8505-DBDE4111F651}"/>
+    <hyperlink ref="B134" r:id="rId133" display="https://www.pgatour.com/players/player.27958.ryan-blaum.html" xr:uid="{27180E2C-871C-FC47-A504-C886676CB519}"/>
+    <hyperlink ref="B135" r:id="rId134" display="https://www.pgatour.com/players/player.31557.jim-herman.html" xr:uid="{38537091-27F3-E84A-BAEA-77C06A1E9551}"/>
+    <hyperlink ref="B136" r:id="rId135" display="https://www.pgatour.com/players/player.32200.roberto-castro.html" xr:uid="{7B5FC4F5-EA4C-D845-84A2-55138770E3CF}"/>
+    <hyperlink ref="B137" r:id="rId136" display="https://www.pgatour.com/players/player.27349.alex-noren.html" xr:uid="{2E4F65C8-B7B7-184D-9A10-9717A3C57EEB}"/>
+    <hyperlink ref="B138" r:id="rId137" display="https://www.pgatour.com/players/player.24924.bill-haas.html" xr:uid="{C5E6B125-35A5-D441-AAB0-16B07538E50E}"/>
+    <hyperlink ref="B139" r:id="rId138" display="https://www.pgatour.com/players/player.33449.zack-sucher.html" xr:uid="{100737EA-80E0-B246-B942-0A2796461722}"/>
+    <hyperlink ref="B140" r:id="rId139" display="https://www.pgatour.com/players/player.40009.dominic-bozzelli.html" xr:uid="{8071FE60-098D-D042-818D-6C7C8679E206}"/>
+    <hyperlink ref="B141" r:id="rId140" display="https://www.pgatour.com/players/player.35461.beau-hossler.html" xr:uid="{3A16AD3A-5EEB-1C4F-BCA2-523250BB7F49}"/>
+    <hyperlink ref="B142" r:id="rId141" display="https://www.pgatour.com/players/player.49766.hank-lebioda.html" xr:uid="{98464727-9D41-8F45-B0D8-1523579B1B8F}"/>
+    <hyperlink ref="B143" r:id="rId142" display="https://www.pgatour.com/players/player.27556.ted-potter--jr-.html" xr:uid="{FF8AA3CB-942C-1346-B321-1554B52C095A}"/>
+    <hyperlink ref="B144" r:id="rId143" display="https://www.pgatour.com/players/player.28252.seamus-power.html" xr:uid="{88EA1517-9164-7040-809E-F8B89CA7AAA7}"/>
+    <hyperlink ref="B145" r:id="rId144" display="https://www.pgatour.com/players/player.34431.robert-streb.html" xr:uid="{6A2C75A2-8F9E-F542-AEE7-FD7785711F63}"/>
+    <hyperlink ref="B146" r:id="rId145" display="https://www.pgatour.com/players/player.36799.stephan-jaeger.html" xr:uid="{8C22E98B-9220-3445-AC2A-610F7A9A3D1A}"/>
+    <hyperlink ref="B147" r:id="rId146" display="https://www.pgatour.com/players/player.29268.bronson-burgoon.html" xr:uid="{6FCB1FE6-6AA7-6843-84E6-C16B56139583}"/>
+    <hyperlink ref="B148" r:id="rId147" display="https://www.pgatour.com/players/player.34261.scott-langley.html" xr:uid="{66BC9C16-0573-B44A-BA5E-6E7233A4A40F}"/>
+    <hyperlink ref="B149" r:id="rId148" display="https://www.pgatour.com/players/player.34099.harris-english.html" xr:uid="{074B5564-510B-DA4D-9C30-C3C97DD70FE4}"/>
+    <hyperlink ref="B150" r:id="rId149" display="https://www.pgatour.com/players/player.27408.martin-kaymer.html" xr:uid="{F73668D5-ABFD-2745-AA6A-A2C68097F71F}"/>
+    <hyperlink ref="B151" r:id="rId150" display="https://www.pgatour.com/players/player.24024.zach-johnson.html" xr:uid="{6EA29EC3-BE9B-5C43-AA7E-B89A238F21EF}"/>
+    <hyperlink ref="B152" r:id="rId151" display="https://www.pgatour.com/players/player.46601.trey-mullinax.html" xr:uid="{47BEB611-CFF5-E04E-95CD-82864488C129}"/>
+    <hyperlink ref="B153" r:id="rId152" display="https://www.pgatour.com/players/player.25632.jimmy-walker.html" xr:uid="{E7FDFDD5-6151-2848-BAF3-374FD0973B84}"/>
+    <hyperlink ref="B154" r:id="rId153" display="https://www.pgatour.com/players/player.24925.jonathan-byrd.html" xr:uid="{2936DC67-E405-D643-BC7D-D533ACF12F45}"/>
+    <hyperlink ref="B155" r:id="rId154" display="https://www.pgatour.com/players/player.49298.kramer-hickok.html" xr:uid="{13589D47-1136-8D49-B70D-62D3407145CD}"/>
+    <hyperlink ref="B156" r:id="rId155" display="https://www.pgatour.com/players/player.34264.hudson-swafford.html" xr:uid="{C636F592-A7AE-DD4F-9FE3-F04989AE2D60}"/>
+    <hyperlink ref="B157" r:id="rId156" display="https://www.pgatour.com/players/player.37340.chase-wright.html" xr:uid="{307BE3F3-99B7-0E44-B4F4-F9C2D3C0E671}"/>
+    <hyperlink ref="B158" r:id="rId157" display="https://www.pgatour.com/players/player.26951.johnson-wagner.html" xr:uid="{19C18D38-36EE-264D-A06E-91AF63FD1FC1}"/>
+    <hyperlink ref="B159" r:id="rId158" display="https://www.pgatour.com/players/player.36852.jim-knous.html" xr:uid="{B49D15E9-CC27-0641-98C7-23D4A8241D4A}"/>
+    <hyperlink ref="B160" r:id="rId159" display="https://www.pgatour.com/players/player.23788.d-j--trahan.html" xr:uid="{21A289D5-37E6-9142-807F-7ADAC3D8C9D0}"/>
+    <hyperlink ref="B161" r:id="rId160" display="https://www.pgatour.com/players/player.45609.tyler-duncan.html" xr:uid="{5A310066-F1B7-B04F-87E1-6AEFFD678E25}"/>
+    <hyperlink ref="B162" r:id="rId161" display="https://www.pgatour.com/players/player.45157.cameron-davis.html" xr:uid="{B934BB12-C13D-DA4F-A425-2E926828CDE9}"/>
+    <hyperlink ref="B163" r:id="rId162" display="https://www.pgatour.com/players/player.30946.alex-prugh.html" xr:uid="{1150E953-6FC7-C040-AC3C-3A7AD02287B8}"/>
+    <hyperlink ref="B164" r:id="rId163" display="https://www.pgatour.com/players/player.46523.joey-garber.html" xr:uid="{E9D97683-B8CB-DE40-B4AD-E7CD3B830A74}"/>
+    <hyperlink ref="B165" r:id="rId164" display="https://www.pgatour.com/players/player.35376.roberto-diaz.html" xr:uid="{5E4FC04F-B377-0D4B-96F8-80E544E31715}"/>
+    <hyperlink ref="B166" r:id="rId165" display="https://www.pgatour.com/players/player.49303.anders-albertson.html" xr:uid="{0ED88A07-9816-F74B-ACD5-D7EAA8DA161B}"/>
+    <hyperlink ref="B167" r:id="rId166" display="https://www.pgatour.com/players/player.40115.adam-svensson.html" xr:uid="{998912B6-A976-8040-9F5E-19A825301D63}"/>
+    <hyperlink ref="B168" r:id="rId167" display="https://www.pgatour.com/players/player.29223.sam-saunders.html" xr:uid="{8FC0B918-A13D-FF44-8BFF-89E1C2C9F8B9}"/>
+    <hyperlink ref="B169" r:id="rId168" display="https://www.pgatour.com/players/player.35421.brandon-harkins.html" xr:uid="{D2A4FB19-8654-3B46-9785-482F314356DB}"/>
+    <hyperlink ref="B170" r:id="rId169" display="https://www.pgatour.com/players/player.29518.brendan-steele.html" xr:uid="{71491BF9-6CE4-FF42-A087-9B7A9F49581F}"/>
+    <hyperlink ref="B171" r:id="rId170" display="https://www.pgatour.com/players/player.26758.david-hearn.html" xr:uid="{932C16C5-95A9-224D-9C95-BDDC35F18C45}"/>
+    <hyperlink ref="B172" r:id="rId171" display="https://www.pgatour.com/players/player.37380.curtis-luck.html" xr:uid="{695A50F8-6176-CE4D-A04B-1B12FA630CF1}"/>
+    <hyperlink ref="B173" r:id="rId172" display="https://www.pgatour.com/players/player.35532.tom-hoge.html" xr:uid="{F86956DD-49BF-0E4F-84BD-D2EBEBAE6470}"/>
+    <hyperlink ref="B174" r:id="rId173" display="https://www.pgatour.com/players/player.30191.julian-etulain.html" xr:uid="{CBD94541-CF27-634B-A43B-FA19687350DF}"/>
+    <hyperlink ref="B175" r:id="rId174" display="https://www.pgatour.com/players/player.27330.josh-teater.html" xr:uid="{08BF37FF-2A73-6A42-904E-69A709532AE4}"/>
+    <hyperlink ref="B176" r:id="rId175" display="https://www.pgatour.com/players/player.32058.jose-de-jesus-rodriguez.html" xr:uid="{5822A767-C270-5F43-8CB5-29BF0039588C}"/>
+    <hyperlink ref="B177" r:id="rId176" display="https://www.pgatour.com/players/player.20229.stewart-cink.html" xr:uid="{5DA4B4E7-C204-6245-BA0B-896AAB6B6CBC}"/>
+    <hyperlink ref="B178" r:id="rId177" display="https://www.pgatour.com/players/player.31420.anirban-lahiri.html" xr:uid="{5BF79EC2-9FAD-D94E-8EDF-51203AD98DAF}"/>
+    <hyperlink ref="B179" r:id="rId178" display="https://www.pgatour.com/players/player.28679.fabian-gomez.html" xr:uid="{BA6EB080-4BC7-1C4F-AB2B-12B7E0CB071E}"/>
+    <hyperlink ref="B180" r:id="rId179" display="https://www.pgatour.com/players/player.46501.ollie-schniederjans.html" xr:uid="{A1CA5127-0909-2947-BE29-B31EF7827558}"/>
+    <hyperlink ref="B181" r:id="rId180" display="https://www.pgatour.com/players/player.39327.ben-silverman.html" xr:uid="{72E5C1A6-4BCB-AA49-973E-2EA88C91FAE5}"/>
+    <hyperlink ref="B182" r:id="rId181" display="https://www.pgatour.com/players/player.06522.ernie-els.html" xr:uid="{71C290DF-B484-8F46-B6BE-E661514C438B}"/>
+    <hyperlink ref="B183" r:id="rId182" display="https://www.pgatour.com/players/player.24781.hunter-mahan.html" xr:uid="{AE174412-AEE3-8245-8C21-760933E2EAE7}"/>
+    <hyperlink ref="B184" r:id="rId183" display="https://www.pgatour.com/players/player.32816.satoshi-kodaira.html" xr:uid="{24BD3475-D262-374D-8324-0230C6C50F68}"/>
+    <hyperlink ref="B185" r:id="rId184" display="https://www.pgatour.com/players/player.30927.brendon-todd.html" xr:uid="{B767FF6B-12CD-F543-8989-FEFDDD0AAD87}"/>
+    <hyperlink ref="B186" r:id="rId185" display="https://www.pgatour.com/players/player.37454.whee-kim.html" xr:uid="{13571EF1-ABEC-9440-87FB-787B701488AC}"/>
+    <hyperlink ref="B187" r:id="rId186" display="https://www.pgatour.com/players/player.47856.seth-reeves.html" xr:uid="{715E0015-7AC6-7D4C-8F6D-B50C78A35B8D}"/>
+    <hyperlink ref="B188" r:id="rId187" display="https://www.pgatour.com/players/player.23983.luke-donald.html" xr:uid="{969317AA-E135-9B40-94C4-2A8A0D66DCF6}"/>
+    <hyperlink ref="B189" r:id="rId188" display="https://www.pgatour.com/players/player.26331.charl-schwartzel.html" xr:uid="{BC8B4D52-7F64-824C-B386-E40AB48D9873}"/>
+    <hyperlink ref="B190" r:id="rId189" display="https://www.pgatour.com/players/player.39954.cody-gribble.html" xr:uid="{2FE52BB8-DF9F-D34F-BAC5-6DB2EC46E274}"/>
+    <hyperlink ref="B191" r:id="rId190" display="https://www.pgatour.com/players/player.32366.kevin-chappell.html" xr:uid="{D91891C7-5BEC-8E4C-847D-6624B77569B4}"/>
+    <hyperlink ref="B192" r:id="rId191" display="https://www.pgatour.com/players/player.01706.davis-love-iii.html" xr:uid="{3FDCEDF1-BF3B-A14B-8CB4-48600727505A}"/>
+    <hyperlink ref="B193" r:id="rId192" display="https://www.pgatour.com/players/player.47990.kyle-jones.html" xr:uid="{CD49ED07-728A-EB44-8ADA-FE0E82170254}"/>
+    <hyperlink ref="B194" r:id="rId193" display="https://www.pgatour.com/players/player.30786.brady-schnell.html" xr:uid="{A520100D-AB2D-B643-B840-4E0F47473449}"/>
+    <hyperlink ref="B195" r:id="rId194" display="https://www.pgatour.com/players/player.29222.billy-hurley-iii.html" xr:uid="{3264D2CE-B12E-AF4C-AEE5-9892A2B65532}"/>
+    <hyperlink ref="B196" r:id="rId195" display="https://www.pgatour.com/players/player.06567.vijay-singh.html" xr:uid="{D3FBDA25-8EC5-024D-B327-154002C1315F}"/>
+    <hyperlink ref="B197" r:id="rId196" display="https://www.pgatour.com/players/player.30926.chris-kirk.html" xr:uid="{E8847A51-7178-3A4E-99D4-C68F9D994296}"/>
+    <hyperlink ref="B198" r:id="rId197" display="https://www.pgatour.com/players/player.23541.ben-crane.html" xr:uid="{CF7FFB1D-9738-B243-AC6F-BC109B306644}"/>
+    <hyperlink ref="B199" r:id="rId198" display="https://www.pgatour.com/players/player.37278.nicholas-lindheim.html" xr:uid="{838AA804-3985-6740-A223-6258C48386F5}"/>
+    <hyperlink ref="B200" r:id="rId199" display="https://www.pgatour.com/players/player.24140.sean-o-hair.html" xr:uid="{584ED7E2-5C65-444A-BE32-2610DEA50323}"/>
+    <hyperlink ref="B201" r:id="rId200" display="https://www.pgatour.com/players/player.23353.j-j--henry.html" xr:uid="{77AEB207-D742-1143-B5DC-0A98F7E5DABA}"/>
+    <hyperlink ref="B202" r:id="rId201" display="https://www.pgatour.com/players/player.28259.sangmoon-bae.html" xr:uid="{C4207E4A-D794-A242-A4E0-D01165937681}"/>
+    <hyperlink ref="B203" r:id="rId202" display="https://www.pgatour.com/players/player.32876.martin-piller.html" xr:uid="{32992557-A0B1-E842-B9C6-002522E7933D}"/>
+    <hyperlink ref="B204" r:id="rId203" display="https://www.pgatour.com/players/player.21731.freddie-jacobson.html" xr:uid="{33ACDD6B-64DC-054D-939E-B11A4191F164}"/>
+    <hyperlink ref="B205" r:id="rId204" display="https://www.pgatour.com/players/player.32448.james-hahn.html" xr:uid="{B5AB3BA7-CFBE-6A44-A6FD-1A6864D99659}"/>
+    <hyperlink ref="B206" r:id="rId205" display="https://www.pgatour.com/players/player.50526.tom-lovelady.html" xr:uid="{4F8A09DD-6E03-404F-91C5-06C504E4480F}"/>
+    <hyperlink ref="B207" r:id="rId206" display="https://www.pgatour.com/players/player.24357.k-j--choi.html" xr:uid="{74A727CA-3F4E-B644-A668-454093A55C00}"/>
+    <hyperlink ref="B208" r:id="rId207" display="https://www.pgatour.com/players/player.29461.jamie-lovemark.html" xr:uid="{5F52F580-BC00-7549-AAF6-635D5E5693A8}"/>
+    <hyperlink ref="B209" r:id="rId208" display="https://www.pgatour.com/players/player.20766.padraig-harrington.html" xr:uid="{810DF5E6-14DE-A44E-8599-DB676C19FCE6}"/>
+    <hyperlink ref="B210" r:id="rId209" display="https://www.pgatour.com/players/player.24490.george-mcneill.html" xr:uid="{16DFE333-C5D0-DE4F-B09A-4AD48C75F5FD}"/>
+    <hyperlink ref="B211" r:id="rId210" display="https://www.pgatour.com/players/player.20472.alex-cejka.html" xr:uid="{E0D8A50C-34B7-A341-B885-32CA796BF92C}"/>
+    <hyperlink ref="B212" r:id="rId211" display="https://www.pgatour.com/players/player.34213.grayson-murray.html" xr:uid="{1DA8B99F-0263-C54C-936C-F31DBFA07603}"/>
+    <hyperlink ref="B213" r:id="rId212" display="https://www.pgatour.com/players/player.28132.tyrone-van-aswegen.html" xr:uid="{E9A80D0C-DF46-604A-AEE0-726E2D1ABB91}"/>
+    <hyperlink ref="B214" r:id="rId213" display="https://www.pgatour.com/players/player.26289.boo-weekley.html" xr:uid="{D4981112-CFD5-7048-8FFC-F762BC43618C}"/>
+    <hyperlink ref="B215" r:id="rId214" display="https://www.pgatour.com/players/player.06527.steve-stricker.html" xr:uid="{B8697D9C-76CA-A443-BEF1-3F266BBCB353}"/>
+    <hyperlink ref="B216" r:id="rId215" display="https://www.pgatour.com/players/player.22892.jason-gore.html" xr:uid="{DFA57DD1-64BE-2D40-9332-C40D90ED4C5C}"/>
+    <hyperlink ref="B217" r:id="rId216" display="https://www.pgatour.com/players/player.31416.derek-fathauer.html" xr:uid="{64FFBEE8-53EB-EC4E-9528-2D3D20FFCE46}"/>
+    <hyperlink ref="B218" r:id="rId217" display="https://www.pgatour.com/players/player.34306.john-chin.html" xr:uid="{21E40824-CBF4-3E42-AFFE-33DEAA624321}"/>
+    <hyperlink ref="B219" r:id="rId218" display="https://www.pgatour.com/players/player.34174.john-huh.html" xr:uid="{9388F195-8C48-8640-8D43-D89F4EC06E5C}"/>
+    <hyperlink ref="B220" r:id="rId219" display="https://www.pgatour.com/players/player.20572.rod-pampling.html" xr:uid="{E6694CCE-AC3B-814A-8C11-48AE33D424C6}"/>
+    <hyperlink ref="B221" r:id="rId220" display="https://www.pgatour.com/players/player.25562.andres-romero.html" xr:uid="{B3CBC3CE-17FC-CA47-9470-C9185135AD5C}"/>
+    <hyperlink ref="B222" r:id="rId221" display="https://www.pgatour.com/players/player.10387.chris-thompson.html" xr:uid="{55F0AABB-D5D7-C04D-90D9-12392E18C863}"/>
+    <hyperlink ref="B223" r:id="rId222" display="https://www.pgatour.com/players/player.02206.david-toms.html" xr:uid="{3B429D12-0F3B-B746-9997-23B7D11DF9F5}"/>
+    <hyperlink ref="B224" r:id="rId223" display="https://www.pgatour.com/players/player.21407.arjun-atwal.html" xr:uid="{0CEC75DF-8C41-3246-8765-A32AF7CD619E}"/>
+    <hyperlink ref="B225" r:id="rId224" display="https://www.pgatour.com/players/player.33461.morgan-hoffmann.html" xr:uid="{0E67AFA4-E030-B142-9266-001C31F3D1C8}"/>
+    <hyperlink ref="B226" r:id="rId225" display="https://www.pgatour.com/players/player.24358.robert-garrigus.html" xr:uid="{18AE477F-6BB3-794D-B973-61B88FFD1537}"/>
+    <hyperlink ref="B227" r:id="rId226" display="https://www.pgatour.com/players/player.39975.michael-kim.html" xr:uid="{B8483872-182E-5F42-88E3-DDADAFAA593D}"/>
+    <hyperlink ref="B228" r:id="rId227" display="https://www.pgatour.com/players/player.20645.john-senden.html" xr:uid="{F34890C9-A838-4A48-A3DC-7083FFC7124E}"/>
+    <hyperlink ref="B229" r:id="rId228" display="https://www.pgatour.com/players/player.30711.colt-knost.html" xr:uid="{3778D94D-09FA-544C-B061-8E7D5CFCB2A7}"/>
+    <hyperlink ref="B230" r:id="rId229" display="https://www.pgatour.com/players/player.34409.david-lingmerth.html" xr:uid="{F518FC9E-1426-0548-B72A-79BE385D4199}"/>
+    <hyperlink ref="B231" r:id="rId230" display="https://www.pgatour.com/players/player.20850.daniel-chopra.html" xr:uid="{5BC752D8-960F-1D4D-AC2E-3290DFFBC276}"/>
+    <hyperlink ref="B232" r:id="rId231" display="https://www.pgatour.com/players/player.24663.y-e--yang.html" xr:uid="{F05FD88E-2A86-AF40-A53E-CBD034D1401F}"/>
+    <hyperlink ref="B233" r:id="rId232" display="https://www.pgatour.com/players/player.24449.parker-mclachlin.html" xr:uid="{49340DE3-4B62-334E-9A09-72EFC1B09BD4}"/>
+    <hyperlink ref="B234" r:id="rId233" display="https://www.pgatour.com/players/player.20098.stuart-appleby.html" xr:uid="{6532F9A8-F53E-9444-BBC8-91C892916C69}"/>
+    <hyperlink ref="B235" r:id="rId234" display="https://www.pgatour.com/players/player.25240.d-a--points.html" xr:uid="{040E4C33-FC4E-D946-8524-C89F08926B65}"/>
+    <hyperlink ref="B236" r:id="rId235" display="https://www.pgatour.com/players/player.11123.chris-couch.html" xr:uid="{231DE5E4-6240-264E-9BF9-515272FDC004}"/>
+    <hyperlink ref="B237" r:id="rId236" display="https://www.pgatour.com/players/player.25720.chad-collins.html" xr:uid="{DEE2EC93-9913-454C-B3D9-E8ECB1F93868}"/>
+    <hyperlink ref="B238" r:id="rId237" display="https://www.pgatour.com/players/player.12510.chad-campbell.html" xr:uid="{D3DAA238-E0BE-3243-805F-CDD4D1E0B0DC}"/>
+    <hyperlink ref="B239" r:id="rId238" display="https://www.pgatour.com/players/player.12782.tim-herron.html" xr:uid="{C34C4DDE-01CF-F44C-8A10-FFF3A8BC688A}"/>
+    <hyperlink ref="B240" r:id="rId239" display="https://www.pgatour.com/players/player.01226.fred-couples.html" xr:uid="{2AB3C635-11AF-C247-9451-CF4E353A616C}"/>
+    <hyperlink ref="B241" r:id="rId240" display="https://www.pgatour.com/players/player.32334.charlie-beljan.html" xr:uid="{E84E5F26-7A40-EE45-B1BC-5B598AB025E8}"/>
+    <hyperlink ref="B242" r:id="rId241" display="https://www.pgatour.com/players/player.22378.trevor-immelman.html" xr:uid="{D843B2D3-A75C-B040-87D8-0584DE921465}"/>
+    <hyperlink ref="B243" r:id="rId242" display="https://www.pgatour.com/players/player.30750.tommy-gainey.html" xr:uid="{E6411AFE-CA31-0B4C-A80C-1F259DA332C2}"/>
+    <hyperlink ref="B244" r:id="rId243" display="https://www.pgatour.com/players/player.24846.ricky-barnes.html" xr:uid="{AEE13F3E-068E-FC4C-96B0-16CAA47701E5}"/>
+    <hyperlink ref="B245" r:id="rId244" display="https://www.pgatour.com/players/player.21753.brian-davis.html" xr:uid="{BC4098A8-97B2-3142-8A9C-AE7B296F5F4D}"/>
+    <hyperlink ref="B246" r:id="rId245" display="https://www.pgatour.com/players/player.27933.john-merrick.html" xr:uid="{95F07858-0F68-4147-9A03-A220D1D438DE}"/>
+    <hyperlink ref="B247" r:id="rId246" display="https://www.pgatour.com/players/player.22913.john-rollins.html" xr:uid="{7603C1B5-9BAF-9042-98CB-FB567B1B4485}"/>
+    <hyperlink ref="B248" r:id="rId247" display="https://www.pgatour.com/players/player.10423.mike-weir.html" xr:uid="{18DEE24D-CAA1-4548-B432-FF0AD9111C24}"/>
+    <hyperlink ref="B249" r:id="rId248" display="https://www.pgatour.com/players/player.01666.bernhard-langer.html" xr:uid="{2DF6AB8B-1859-4E46-96FC-4146BA50871B}"/>
+    <hyperlink ref="B250" r:id="rId249" display="https://www.pgatour.com/players/player.10885.robert-allenby.html" xr:uid="{14B70594-23AA-5E42-B839-911F3C73DF00}"/>
+    <hyperlink ref="B251" r:id="rId250" display="https://www.pgatour.com/players/player.01677.tom-lehman.html" xr:uid="{F317FD42-8EDC-B44B-8E46-393A329A3879}"/>
+    <hyperlink ref="B252" r:id="rId251" display="https://www.pgatour.com/players/player.37273.derek-ernst.html" xr:uid="{E1FD9C5F-20BC-C540-A7D8-89191E0A69B7}"/>
+    <hyperlink ref="B253" r:id="rId252" display="https://www.pgatour.com/players/player.46550.brandon-hagy.html" xr:uid="{A491E052-8DF7-B24E-BD0B-95A144FDA3F2}"/>
+    <hyperlink ref="B254" r:id="rId253" display="https://www.pgatour.com/players/player.20160.charlie-wi.html" xr:uid="{BAD025EE-4DF1-3741-87A9-4858B2F28A21}"/>
+    <hyperlink ref="B255" r:id="rId254" display="https://www.pgatour.com/players/player.46440.smylie-kaufman.html" xr:uid="{13F1B2FE-2FCC-A944-B2B4-EFFFFE7422F0}"/>
+    <hyperlink ref="B256" r:id="rId255" display="https://www.pgatour.com/players/player.20104.ken-duke.html" xr:uid="{57964516-9F21-6B44-A246-471CD77629C8}"/>
+    <hyperlink ref="B257" r:id="rId256" display="https://www.pgatour.com/players/player.10213.dicky-pride.html" xr:uid="{B54F6945-F39E-874A-9A6C-6C0E8ECF787D}"/>
+    <hyperlink ref="B258" r:id="rId257" display="https://www.pgatour.com/players/player.23614.rich-beem.html" xr:uid="{C1E140DD-5224-0043-9B57-FA8FAC6ACBBB}"/>
+    <hyperlink ref="B259" r:id="rId258" display="https://www.pgatour.com/players/player.23638.brendon-de-jonge.html" xr:uid="{7EA6DDDE-BB1D-C24D-BFF4-D04993955314}"/>
+    <hyperlink ref="B260" r:id="rId259" display="https://www.pgatour.com/players/player.24507.jason-bohn.html" xr:uid="{A685A22D-ABE0-AB42-B155-8B9A6207914D}"/>
+    <hyperlink ref="B261" r:id="rId260" display="https://www.pgatour.com/players/player.20094.jonathan-kaye.html" xr:uid="{D17FF988-14FD-A54E-8570-4696B9A42230}"/>
+    <hyperlink ref="B262" r:id="rId261" display="https://www.pgatour.com/players/player.08385.omar-uresti.html" xr:uid="{E00BC68D-828D-D747-B206-4394BC798254}"/>
+    <hyperlink ref="B263" r:id="rId262" display="https://www.pgatour.com/players/player.22293.heath-slocum.html" xr:uid="{B3FA127F-C494-A24F-A173-861F0CDF341C}"/>
+    <hyperlink ref="B264" r:id="rId263" display="https://www.pgatour.com/players/player.24912.will-mackenzie.html" xr:uid="{FB938456-78C2-0540-8A49-57A786EB6E21}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Got the remaining custom commands to load data into the db working
</commit_message>
<xml_diff>
--- a/fg/external_files/players.xlsx
+++ b/fg/external_files/players.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexevans/Library/Containers/com.microsoft.Excel/Data/Desktop/Projects/fgolf/fg/external_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{108924EB-F1A9-6C4A-9297-9303A52FADE4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2A2CDDA-5658-584D-9D76-B7B177947291}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="15920" xr2:uid="{11440A6E-CB72-CD4F-877F-52107475F245}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="267">
   <si>
     <t>PLAYER NAME</t>
   </si>
@@ -829,6 +829,9 @@
   </si>
   <si>
     <t>Erik van Rooyen</t>
+  </si>
+  <si>
+    <t>Thorbjorn Olesen</t>
   </si>
 </sst>
 </file>
@@ -1202,7 +1205,7 @@
   <dimension ref="A1:B266"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A248" workbookViewId="0">
-      <selection activeCell="E270" sqref="E270"/>
+      <selection activeCell="A266" sqref="A266"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3326,7 +3329,7 @@
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A265" s="2" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="B265" s="2" t="s">
         <v>264</v>

</xml_diff>